<commit_message>
Updated with SIQ's added
</commit_message>
<xml_diff>
--- a/Lhub_RTM.xlsx
+++ b/Lhub_RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Desktop\V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazmy\Documents\GitHub\Learning-hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -368,6 +368,22 @@
 Lhub_SDD_6.1.6.2.2
 Lhub_SDD_5.2.5
 Lhub_SDD_5.2.6</t>
+  </si>
+  <si>
+    <t>SIQ_37</t>
+  </si>
+  <si>
+    <t>SIQ_38</t>
+  </si>
+  <si>
+    <t>SIQ_39
+SIQ_40</t>
+  </si>
+  <si>
+    <t>SIQ_41</t>
+  </si>
+  <si>
+    <t>SIQ_42</t>
   </si>
 </sst>
 </file>
@@ -616,7 +632,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -746,10 +762,59 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -758,92 +823,46 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1173,21 +1192,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="48.1796875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="35.81640625" style="12" customWidth="1"/>
     <col min="6" max="6" width="38" style="22" customWidth="1"/>
-    <col min="7" max="7" width="37.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="44.5703125" style="12" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="12"/>
+    <col min="7" max="7" width="37.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="44.54296875" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="4" customFormat="1" ht="30" customHeight="1">
@@ -1200,10 +1219,10 @@
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="58"/>
+      <c r="C2" s="70"/>
       <c r="D2" s="23" t="s">
         <v>61</v>
       </c>
@@ -1224,10 +1243,10 @@
       <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="70"/>
       <c r="D3" s="24" t="s">
         <v>66</v>
       </c>
@@ -1248,10 +1267,10 @@
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="71">
         <v>43470</v>
       </c>
-      <c r="C4" s="59"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="25"/>
       <c r="E4" s="14">
         <v>43592</v>
@@ -1264,7 +1283,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="7" customFormat="1" ht="25.5">
+    <row r="5" spans="1:26" s="7" customFormat="1" ht="25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1309,22 +1328,22 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" s="9" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A6" s="49">
+      <c r="A6" s="66">
         <v>1</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="65" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="50"/>
+      <c r="D6" s="67"/>
       <c r="E6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="60"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="69"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -1345,18 +1364,18 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" spans="1:26" s="9" customFormat="1">
-      <c r="A7" s="49"/>
-      <c r="B7" s="53"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="50"/>
+      <c r="D7" s="67"/>
       <c r="E7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="60"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="69"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1405,24 +1424,24 @@
       <c r="Z8" s="34"/>
     </row>
     <row r="9" spans="1:26" s="9" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="49">
+      <c r="A9" s="66">
         <v>2</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="65" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="50"/>
+      <c r="D9" s="67"/>
       <c r="E9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="G9" s="65"/>
-      <c r="H9" s="49"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="66"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1443,18 +1462,18 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A10" s="49"/>
-      <c r="B10" s="53"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="50"/>
+      <c r="D10" s="67"/>
       <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="52"/>
+      <c r="F10" s="73"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="49"/>
+      <c r="H10" s="66"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1475,16 +1494,16 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="49"/>
-      <c r="B11" s="53"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="50"/>
+      <c r="D11" s="67"/>
       <c r="E11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="52"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="8"/>
@@ -1507,16 +1526,16 @@
       <c r="Z11" s="8"/>
     </row>
     <row r="12" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="49"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="50"/>
+      <c r="D12" s="67"/>
       <c r="E12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="52"/>
+      <c r="F12" s="73"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="8"/>
@@ -1539,14 +1558,16 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="49"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="50"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="67"/>
       <c r="E13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="52"/>
+      <c r="F13" s="73"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="8"/>
@@ -1569,14 +1590,14 @@
       <c r="Z13" s="8"/>
     </row>
     <row r="14" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="49"/>
-      <c r="B14" s="53"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="39"/>
-      <c r="D14" s="50"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="52"/>
+      <c r="F14" s="73"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="8"/>
@@ -1599,14 +1620,14 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="49"/>
-      <c r="B15" s="53"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="39"/>
-      <c r="D15" s="50"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="52"/>
+      <c r="F15" s="73"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="8"/>
@@ -1629,14 +1650,14 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="49"/>
-      <c r="B16" s="53"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="39"/>
-      <c r="D16" s="50"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="52"/>
+      <c r="F16" s="73"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="8"/>
@@ -1659,14 +1680,14 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="49"/>
-      <c r="B17" s="53"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="39"/>
-      <c r="D17" s="50"/>
+      <c r="D17" s="67"/>
       <c r="E17" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="52"/>
+      <c r="F17" s="73"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="8"/>
@@ -1689,14 +1710,14 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="49"/>
-      <c r="B18" s="53"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="65"/>
       <c r="C18" s="39"/>
-      <c r="D18" s="50"/>
+      <c r="D18" s="67"/>
       <c r="E18" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="52"/>
+      <c r="F18" s="73"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="8"/>
@@ -1719,14 +1740,14 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="39"/>
-      <c r="D19" s="50"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="52"/>
+      <c r="F19" s="73"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="8"/>
@@ -1749,14 +1770,14 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="49"/>
-      <c r="B20" s="53"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="39"/>
-      <c r="D20" s="50"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="52"/>
+      <c r="F20" s="73"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="8"/>
@@ -1779,14 +1800,14 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="49"/>
-      <c r="B21" s="53"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="39"/>
-      <c r="D21" s="50"/>
+      <c r="D21" s="67"/>
       <c r="E21" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="52"/>
+      <c r="F21" s="73"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="8"/>
@@ -1809,14 +1830,14 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="49"/>
-      <c r="B22" s="53"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="39"/>
-      <c r="D22" s="50"/>
+      <c r="D22" s="67"/>
       <c r="E22" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="52"/>
+      <c r="F22" s="73"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="8"/>
@@ -1839,14 +1860,14 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="49"/>
-      <c r="B23" s="53"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="39"/>
-      <c r="D23" s="50"/>
+      <c r="D23" s="67"/>
       <c r="E23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="52"/>
+      <c r="F23" s="73"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="8"/>
@@ -1869,14 +1890,14 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="49"/>
-      <c r="B24" s="53"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="39"/>
-      <c r="D24" s="50"/>
+      <c r="D24" s="67"/>
       <c r="E24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="52"/>
+      <c r="F24" s="73"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="8"/>
@@ -1899,14 +1920,14 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A25" s="49"/>
-      <c r="B25" s="53"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="65"/>
       <c r="C25" s="39"/>
-      <c r="D25" s="50"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="52"/>
+      <c r="F25" s="73"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="8"/>
@@ -1929,14 +1950,14 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="49"/>
-      <c r="B26" s="53"/>
+      <c r="A26" s="66"/>
+      <c r="B26" s="65"/>
       <c r="C26" s="39"/>
-      <c r="D26" s="50"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="52"/>
+      <c r="F26" s="73"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="8"/>
@@ -1959,14 +1980,14 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="49"/>
-      <c r="B27" s="53"/>
+      <c r="A27" s="66"/>
+      <c r="B27" s="65"/>
       <c r="C27" s="39"/>
-      <c r="D27" s="50"/>
+      <c r="D27" s="67"/>
       <c r="E27" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="52"/>
+      <c r="F27" s="73"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="8"/>
@@ -2235,7 +2256,7 @@
       <c r="D36" s="32"/>
       <c r="E36" s="33"/>
       <c r="F36" s="36"/>
-      <c r="G36" s="68"/>
+      <c r="G36" s="51"/>
       <c r="H36" s="37"/>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
@@ -2269,7 +2290,7 @@
       <c r="E37" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="55" t="s">
+      <c r="F37" s="56" t="s">
         <v>97</v>
       </c>
       <c r="G37" s="40"/>
@@ -2302,7 +2323,7 @@
       <c r="E38" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="69"/>
+      <c r="F38" s="82"/>
       <c r="G38" s="40"/>
       <c r="H38" s="11"/>
       <c r="I38" s="8"/>
@@ -2333,7 +2354,7 @@
       <c r="E39" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F39" s="69"/>
+      <c r="F39" s="82"/>
       <c r="G39" s="40"/>
       <c r="H39" s="11"/>
       <c r="I39" s="8"/>
@@ -2365,7 +2386,7 @@
       <c r="E40" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F40" s="69"/>
+      <c r="F40" s="82"/>
       <c r="G40" s="40"/>
       <c r="H40" s="11"/>
       <c r="I40" s="8"/>
@@ -2397,7 +2418,7 @@
       <c r="E41" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="F41" s="70"/>
+      <c r="F41" s="83"/>
       <c r="G41" s="40"/>
       <c r="H41" s="11"/>
       <c r="I41" s="8"/>
@@ -2422,7 +2443,9 @@
     <row r="42" spans="1:26" s="45" customFormat="1" ht="27" customHeight="1">
       <c r="A42" s="40"/>
       <c r="B42" s="42"/>
-      <c r="C42" s="44"/>
+      <c r="C42" s="47" t="s">
+        <v>107</v>
+      </c>
       <c r="D42" s="44"/>
       <c r="E42" s="28" t="s">
         <v>53</v>
@@ -2480,7 +2503,7 @@
       <c r="Z43" s="34"/>
     </row>
     <row r="44" spans="1:26" s="45" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A44" s="61">
+      <c r="A44" s="59">
         <v>4</v>
       </c>
       <c r="B44" s="62" t="s">
@@ -2489,11 +2512,11 @@
       <c r="C44" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="80"/>
+      <c r="D44" s="74"/>
       <c r="E44" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="F44" s="55" t="s">
+      <c r="F44" s="56" t="s">
         <v>102</v>
       </c>
       <c r="G44" s="11" t="s">
@@ -2519,47 +2542,47 @@
       <c r="Y44" s="8"/>
       <c r="Z44" s="8"/>
     </row>
-    <row r="45" spans="1:26" s="74" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A45" s="47"/>
+    <row r="45" spans="1:26" s="55" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A45" s="60"/>
       <c r="B45" s="63"/>
-      <c r="C45" s="71" t="s">
+      <c r="C45" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="81"/>
-      <c r="E45" s="72" t="s">
+      <c r="D45" s="75"/>
+      <c r="E45" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="F45" s="69"/>
-      <c r="G45" s="66"/>
-      <c r="H45" s="66"/>
-      <c r="I45" s="73"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="73"/>
-      <c r="L45" s="73"/>
-      <c r="M45" s="73"/>
-      <c r="N45" s="73"/>
-      <c r="O45" s="73"/>
-      <c r="P45" s="73"/>
-      <c r="Q45" s="73"/>
-      <c r="R45" s="73"/>
-      <c r="S45" s="73"/>
-      <c r="T45" s="73"/>
-      <c r="U45" s="73"/>
-      <c r="V45" s="73"/>
-      <c r="W45" s="73"/>
-      <c r="X45" s="73"/>
-      <c r="Y45" s="73"/>
-      <c r="Z45" s="73"/>
+      <c r="F45" s="82"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="54"/>
+      <c r="K45" s="54"/>
+      <c r="L45" s="54"/>
+      <c r="M45" s="54"/>
+      <c r="N45" s="54"/>
+      <c r="O45" s="54"/>
+      <c r="P45" s="54"/>
+      <c r="Q45" s="54"/>
+      <c r="R45" s="54"/>
+      <c r="S45" s="54"/>
+      <c r="T45" s="54"/>
+      <c r="U45" s="54"/>
+      <c r="V45" s="54"/>
+      <c r="W45" s="54"/>
+      <c r="X45" s="54"/>
+      <c r="Y45" s="54"/>
+      <c r="Z45" s="54"/>
     </row>
     <row r="46" spans="1:26" s="45" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A46" s="47"/>
+      <c r="A46" s="60"/>
       <c r="B46" s="63"/>
       <c r="C46" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="81"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="69"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="79"/>
+      <c r="F46" s="82"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="8"/>
@@ -2582,12 +2605,12 @@
       <c r="Z46" s="8"/>
     </row>
     <row r="47" spans="1:26" s="45" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A47" s="47"/>
+      <c r="A47" s="60"/>
       <c r="B47" s="63"/>
-      <c r="C47" s="78"/>
-      <c r="D47" s="81"/>
-      <c r="E47" s="76"/>
-      <c r="F47" s="69"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="80"/>
+      <c r="F47" s="82"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="8"/>
@@ -2610,12 +2633,12 @@
       <c r="Z47" s="8"/>
     </row>
     <row r="48" spans="1:26" s="45" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A48" s="48"/>
+      <c r="A48" s="61"/>
       <c r="B48" s="64"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="77"/>
-      <c r="F48" s="70"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="81"/>
+      <c r="F48" s="83"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="8"/>
@@ -2666,10 +2689,10 @@
       <c r="Z49" s="34"/>
     </row>
     <row r="50" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A50" s="49">
+      <c r="A50" s="66">
         <v>5</v>
       </c>
-      <c r="B50" s="53" t="s">
+      <c r="B50" s="65" t="s">
         <v>36</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2678,7 +2701,7 @@
       <c r="E50" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F50" s="55" t="s">
+      <c r="F50" s="56" t="s">
         <v>103</v>
       </c>
       <c r="G50" s="40"/>
@@ -2703,13 +2726,13 @@
       <c r="Z50" s="8"/>
     </row>
     <row r="51" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A51" s="49"/>
-      <c r="B51" s="53"/>
+      <c r="A51" s="66"/>
+      <c r="B51" s="65"/>
       <c r="C51" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E51" s="10"/>
-      <c r="F51" s="56"/>
+      <c r="F51" s="57"/>
       <c r="G51" s="46"/>
       <c r="H51" s="11"/>
       <c r="I51" s="8"/>
@@ -2732,13 +2755,13 @@
       <c r="Z51" s="8"/>
     </row>
     <row r="52" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A52" s="49"/>
-      <c r="B52" s="53"/>
+      <c r="A52" s="66"/>
+      <c r="B52" s="65"/>
       <c r="C52" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E52" s="10"/>
-      <c r="F52" s="57"/>
+      <c r="F52" s="58"/>
       <c r="G52" s="40"/>
       <c r="H52" s="11"/>
       <c r="I52" s="8"/>
@@ -2789,20 +2812,20 @@
       <c r="Z53" s="34"/>
     </row>
     <row r="54" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="49">
+      <c r="A54" s="66">
         <v>6</v>
       </c>
-      <c r="B54" s="53" t="s">
+      <c r="B54" s="65" t="s">
         <v>37</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D54" s="50"/>
+      <c r="D54" s="67"/>
       <c r="E54" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F54" s="55" t="s">
+      <c r="F54" s="56" t="s">
         <v>104</v>
       </c>
       <c r="G54" s="40"/>
@@ -2827,14 +2850,14 @@
       <c r="Z54" s="8"/>
     </row>
     <row r="55" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A55" s="49"/>
-      <c r="B55" s="53"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="50"/>
+      <c r="A55" s="66"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="67"/>
       <c r="E55" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F55" s="56"/>
+      <c r="F55" s="57"/>
       <c r="G55" s="46"/>
       <c r="H55" s="11"/>
       <c r="I55" s="8"/>
@@ -2857,14 +2880,14 @@
       <c r="Z55" s="8"/>
     </row>
     <row r="56" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A56" s="49"/>
-      <c r="B56" s="53"/>
-      <c r="C56" s="54"/>
-      <c r="D56" s="50"/>
+      <c r="A56" s="66"/>
+      <c r="B56" s="65"/>
+      <c r="C56" s="68"/>
+      <c r="D56" s="67"/>
       <c r="E56" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F56" s="57"/>
+      <c r="F56" s="58"/>
       <c r="G56" s="46"/>
       <c r="H56" s="11"/>
       <c r="I56" s="8"/>
@@ -2921,7 +2944,9 @@
       <c r="B58" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C58" s="3"/>
+      <c r="C58" s="47" t="s">
+        <v>109</v>
+      </c>
       <c r="D58" s="19"/>
       <c r="E58" s="13" t="s">
         <v>55</v>
@@ -2979,7 +3004,7 @@
       <c r="Z59" s="34"/>
     </row>
     <row r="60" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A60" s="61">
+      <c r="A60" s="59">
         <v>8</v>
       </c>
       <c r="B60" s="62" t="s">
@@ -2992,7 +3017,7 @@
       <c r="E60" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F60" s="55" t="s">
+      <c r="F60" s="56" t="s">
         <v>106</v>
       </c>
       <c r="G60" s="46"/>
@@ -3017,14 +3042,16 @@
       <c r="Z60" s="8"/>
     </row>
     <row r="61" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A61" s="47"/>
+      <c r="A61" s="60"/>
       <c r="B61" s="63"/>
-      <c r="C61" s="3"/>
+      <c r="C61" s="47" t="s">
+        <v>110</v>
+      </c>
       <c r="D61" s="19"/>
       <c r="E61" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F61" s="56"/>
+      <c r="F61" s="57"/>
       <c r="G61" s="46"/>
       <c r="H61" s="11"/>
       <c r="I61" s="8"/>
@@ -3047,14 +3074,16 @@
       <c r="Z61" s="8"/>
     </row>
     <row r="62" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A62" s="47"/>
+      <c r="A62" s="60"/>
       <c r="B62" s="63"/>
-      <c r="C62" s="3"/>
+      <c r="C62" s="47" t="s">
+        <v>111</v>
+      </c>
       <c r="D62" s="19"/>
       <c r="E62" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F62" s="56"/>
+      <c r="F62" s="57"/>
       <c r="G62" s="40"/>
       <c r="H62" s="11"/>
       <c r="I62" s="8"/>
@@ -3077,14 +3106,14 @@
       <c r="Z62" s="8"/>
     </row>
     <row r="63" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A63" s="48"/>
+      <c r="A63" s="61"/>
       <c r="B63" s="64"/>
       <c r="C63" s="3"/>
       <c r="D63" s="19"/>
       <c r="E63" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F63" s="57"/>
+      <c r="F63" s="58"/>
       <c r="G63" s="40"/>
       <c r="H63" s="11"/>
       <c r="I63" s="8"/>
@@ -3172,6 +3201,26 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="F44:F48"/>
+    <mergeCell ref="F37:F41"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B27"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A9:A27"/>
+    <mergeCell ref="D9:D27"/>
+    <mergeCell ref="F9:F27"/>
     <mergeCell ref="F50:F52"/>
     <mergeCell ref="F54:F56"/>
     <mergeCell ref="F60:F63"/>
@@ -3183,26 +3232,6 @@
     <mergeCell ref="A50:A52"/>
     <mergeCell ref="B50:B52"/>
     <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B27"/>
-    <mergeCell ref="A9:A27"/>
-    <mergeCell ref="D9:D27"/>
-    <mergeCell ref="F9:F27"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="D44:D48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F44:F48"/>
-    <mergeCell ref="F37:F41"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
Edit the RTM in column architecture design with class digrams ID
</commit_message>
<xml_diff>
--- a/Lhub_RTM.xlsx
+++ b/Lhub_RTM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -321,94 +321,53 @@
     <t>Aya</t>
   </si>
   <si>
+    <t>Lhub_SDD_4.1.3
+Lhub_SDD_5.2.9</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_5.2.4</t>
+  </si>
+  <si>
     <t>Lhub_SDD_4.1.1
 Lhub_SDD_5.2.1
-Lhub_SDD_5.2.2</t>
+Lhub_SDD_5.2.2
+Lhub_SDD_6.1.7.2.1
+Lhub_SDD_6.1.7.2.2
+Lhub_SDD_6.1.7.2.3
+Lhub_SDD_6.1.7.2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lhub_SDD_6.1.2.2.3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lhub_SDD_6.1.5.2.5 
+Lhub_SDD_4.1.3
+Lhub_SDD_5.2.9</t>
   </si>
   <si>
     <t>Lhub_SDD_4.1.3
+Lhub_SDD_6.1.5.2.6
 Lhub_SDD_5.2.9</t>
   </si>
   <si>
     <t>Lhub_SDD_4.1.4
-Lhub_SDD_5.2.3</t>
+Lhub_SDD_5.2.3
+Lhub_SDD__6.1.2.2.3
+Lhub_SDD__6.1.2.2.4</t>
   </si>
   <si>
     <t>Lhub_SDD_4.1.2
-Lhub_SDD_5.2.4</t>
-  </si>
-  <si>
-    <t>Lhub_SDD_5.2.4</t>
-  </si>
-  <si>
-    <t>Lhub_SDD_5.2.5
+Lhub_SDD_5.2.4
+Lhub_SDD_6.1.2.2.6</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_6.1.3.2.1
+Lhub_SDD_6.1.6.2.2
+Lhub_SDD_5.2.5
 Lhub_SDD_5.2.6</t>
-  </si>
-  <si>
-    <t>Lhub_ClassDigram_6.1.7.2.1
-Lhub_ClassDigram_6.1.7.2.2
-Lhub_ClassDigram_6.1.7.2.3
-Lhub_ClassDigram_6.1.7.2.4</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>Lhub_classDigam_6.1.2.2.3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>Lhub_ClassDigram_6.1.2.2.3</t>
-  </si>
-  <si>
-    <t>Lhub_ClassDigram_6.1.2.2.4</t>
-  </si>
-  <si>
-    <t>Lhub_ClassDigram_6.1.2.2.6</t>
-  </si>
-  <si>
-    <t>Lhub_ClassDigram_6.1.3.2.1</t>
-  </si>
-  <si>
-    <t>Lhub_ClassDigram_6.1.6.2.2</t>
-  </si>
-  <si>
-    <t>Lhub_ClassDihram_6.1.5.2.6</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">          </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  Lhub_ClassDigram_6.1.5.2.5 </t>
-    </r>
   </si>
 </sst>
 </file>
@@ -657,7 +616,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -762,15 +721,55 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -780,60 +779,72 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1162,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:G36"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1189,10 +1200,10 @@
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="53"/>
+      <c r="C2" s="58"/>
       <c r="D2" s="23" t="s">
         <v>61</v>
       </c>
@@ -1213,10 +1224,10 @@
       <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="53"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="24" t="s">
         <v>66</v>
       </c>
@@ -1237,10 +1248,10 @@
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="59">
         <v>43470</v>
       </c>
-      <c r="C4" s="54"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="25"/>
       <c r="E4" s="14">
         <v>43592</v>
@@ -1298,22 +1309,22 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" s="9" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A6" s="50">
+      <c r="A6" s="49">
         <v>1</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="53" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="51"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="60"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -1334,18 +1345,18 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" spans="1:26" s="9" customFormat="1">
-      <c r="A7" s="50"/>
-      <c r="B7" s="55"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="51"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="60"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1394,26 +1405,24 @@
       <c r="Z8" s="34"/>
     </row>
     <row r="9" spans="1:26" s="9" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="50">
+      <c r="A9" s="49">
         <v>2</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="53" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="51"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="G9" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="H9" s="50"/>
+      <c r="F9" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="65"/>
+      <c r="H9" s="49"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1434,18 +1443,18 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A10" s="50"/>
-      <c r="B10" s="55"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="51"/>
+      <c r="D10" s="50"/>
       <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="50"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="49"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1466,17 +1475,17 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="50"/>
-      <c r="B11" s="55"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="50"/>
       <c r="E11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="45"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -1498,17 +1507,17 @@
       <c r="Z11" s="8"/>
     </row>
     <row r="12" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="50"/>
-      <c r="B12" s="55"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="51"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="45"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -1530,15 +1539,15 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="50"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="51"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="45"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -1560,15 +1569,15 @@
       <c r="Z13" s="8"/>
     </row>
     <row r="14" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="50"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="51"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="57"/>
-      <c r="G14" s="45"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -1590,15 +1599,15 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="50"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="51"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="45"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -1620,15 +1629,15 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="50"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="51"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="45"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -1650,15 +1659,15 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="50"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="51"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="45"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -1680,15 +1689,15 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="50"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="51"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="45"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1710,15 +1719,15 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="50"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="51"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="45"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -1740,15 +1749,15 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="50"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="51"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="45"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -1770,15 +1779,15 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="50"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="51"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="45"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -1800,15 +1809,15 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="50"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="51"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="57"/>
-      <c r="G22" s="45"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -1830,15 +1839,15 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="50"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="51"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="50"/>
       <c r="E23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="57"/>
-      <c r="G23" s="45"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -1860,15 +1869,15 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="50"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="51"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="57"/>
-      <c r="G24" s="45"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -1890,15 +1899,15 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A25" s="50"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="51"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="50"/>
       <c r="E25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="57"/>
-      <c r="G25" s="45"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -1920,15 +1929,15 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="50"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="51"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="57"/>
-      <c r="G26" s="45"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
@@ -1950,15 +1959,15 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="50"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="51"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="57"/>
-      <c r="G27" s="45"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
@@ -1988,7 +1997,7 @@
         <v>81</v>
       </c>
       <c r="F28" s="21"/>
-      <c r="G28" s="45"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -2018,7 +2027,7 @@
         <v>82</v>
       </c>
       <c r="F29" s="21"/>
-      <c r="G29" s="45"/>
+      <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
@@ -2048,7 +2057,7 @@
         <v>83</v>
       </c>
       <c r="F30" s="21"/>
-      <c r="G30" s="45"/>
+      <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
@@ -2078,7 +2087,7 @@
         <v>84</v>
       </c>
       <c r="F31" s="21"/>
-      <c r="G31" s="45"/>
+      <c r="G31" s="11"/>
       <c r="H31" s="11"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
@@ -2108,7 +2117,7 @@
         <v>85</v>
       </c>
       <c r="F32" s="21"/>
-      <c r="G32" s="45"/>
+      <c r="G32" s="11"/>
       <c r="H32" s="11"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
@@ -2138,7 +2147,7 @@
         <v>86</v>
       </c>
       <c r="F33" s="21"/>
-      <c r="G33" s="45"/>
+      <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
@@ -2168,7 +2177,7 @@
         <v>87</v>
       </c>
       <c r="F34" s="21"/>
-      <c r="G34" s="45"/>
+      <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
@@ -2198,7 +2207,7 @@
         <v>88</v>
       </c>
       <c r="F35" s="21"/>
-      <c r="G35" s="45"/>
+      <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
@@ -2226,7 +2235,7 @@
       <c r="D36" s="32"/>
       <c r="E36" s="33"/>
       <c r="F36" s="36"/>
-      <c r="G36" s="46"/>
+      <c r="G36" s="68"/>
       <c r="H36" s="37"/>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
@@ -2247,23 +2256,23 @@
       <c r="Y36" s="34"/>
       <c r="Z36" s="34"/>
     </row>
-    <row r="37" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A37" s="50">
+    <row r="37" spans="1:26" s="45" customFormat="1" ht="27" customHeight="1">
+      <c r="A37" s="40">
         <v>3</v>
       </c>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="44" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="G37" s="18"/>
+      <c r="F37" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" s="40"/>
       <c r="H37" s="11"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
@@ -2284,17 +2293,17 @@
       <c r="Y37" s="8"/>
       <c r="Z37" s="8"/>
     </row>
-    <row r="38" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A38" s="50"/>
-      <c r="B38" s="55"/>
-      <c r="C38" s="3" t="s">
+    <row r="38" spans="1:26" s="45" customFormat="1" ht="27" customHeight="1">
+      <c r="A38" s="40"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="44" t="s">
         <v>20</v>
       </c>
       <c r="E38" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="42"/>
-      <c r="G38" s="18"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="40"/>
       <c r="H38" s="11"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
@@ -2315,17 +2324,17 @@
       <c r="Y38" s="8"/>
       <c r="Z38" s="8"/>
     </row>
-    <row r="39" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A39" s="50"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="3" t="s">
+    <row r="39" spans="1:26" s="45" customFormat="1" ht="27" customHeight="1">
+      <c r="A39" s="40"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="44" t="s">
         <v>21</v>
       </c>
       <c r="E39" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F39" s="42"/>
-      <c r="G39" s="18"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="40"/>
       <c r="H39" s="11"/>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
@@ -2346,18 +2355,18 @@
       <c r="Y39" s="8"/>
       <c r="Z39" s="8"/>
     </row>
-    <row r="40" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A40" s="50"/>
-      <c r="B40" s="55"/>
-      <c r="C40" s="3" t="s">
+    <row r="40" spans="1:26" s="45" customFormat="1" ht="27" customHeight="1">
+      <c r="A40" s="40"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="44"/>
       <c r="E40" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F40" s="42"/>
-      <c r="G40" s="18"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="40"/>
       <c r="H40" s="11"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
@@ -2378,18 +2387,18 @@
       <c r="Y40" s="8"/>
       <c r="Z40" s="8"/>
     </row>
-    <row r="41" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A41" s="50"/>
-      <c r="B41" s="55"/>
-      <c r="C41" s="3" t="s">
+    <row r="41" spans="1:26" s="45" customFormat="1" ht="27" customHeight="1">
+      <c r="A41" s="40"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="44"/>
       <c r="E41" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="F41" s="42"/>
-      <c r="G41" s="18"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="40"/>
       <c r="H41" s="11"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
@@ -2410,18 +2419,18 @@
       <c r="Y41" s="8"/>
       <c r="Z41" s="8"/>
     </row>
-    <row r="42" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A42" s="18"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+    <row r="42" spans="1:26" s="45" customFormat="1" ht="27" customHeight="1">
+      <c r="A42" s="40"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
       <c r="E42" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="43"/>
-      <c r="G42" s="18" t="s">
-        <v>104</v>
-      </c>
+      <c r="F42" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42" s="40"/>
       <c r="H42" s="11"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
@@ -2470,25 +2479,25 @@
       <c r="Y43" s="34"/>
       <c r="Z43" s="34"/>
     </row>
-    <row r="44" spans="1:26" s="9" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A44" s="50">
+    <row r="44" spans="1:26" s="45" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A44" s="61">
         <v>4</v>
       </c>
-      <c r="B44" s="55" t="s">
+      <c r="B44" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="51"/>
-      <c r="E44" s="10" t="s">
+      <c r="D44" s="80"/>
+      <c r="E44" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="F44" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="G44" s="62" t="s">
-        <v>111</v>
+      <c r="F44" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="H44" s="11"/>
       <c r="I44" s="8"/>
@@ -2510,47 +2519,47 @@
       <c r="Y44" s="8"/>
       <c r="Z44" s="8"/>
     </row>
-    <row r="45" spans="1:26" s="9" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A45" s="50"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="3" t="s">
+    <row r="45" spans="1:26" s="74" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A45" s="47"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="51"/>
-      <c r="E45" s="10" t="s">
+      <c r="D45" s="81"/>
+      <c r="E45" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="F45" s="42"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="8"/>
-      <c r="T45" s="8"/>
-      <c r="U45" s="8"/>
-      <c r="V45" s="8"/>
-      <c r="W45" s="8"/>
-      <c r="X45" s="8"/>
-      <c r="Y45" s="8"/>
-      <c r="Z45" s="8"/>
-    </row>
-    <row r="46" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A46" s="50"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="3" t="s">
+      <c r="F45" s="69"/>
+      <c r="G45" s="66"/>
+      <c r="H45" s="66"/>
+      <c r="I45" s="73"/>
+      <c r="J45" s="73"/>
+      <c r="K45" s="73"/>
+      <c r="L45" s="73"/>
+      <c r="M45" s="73"/>
+      <c r="N45" s="73"/>
+      <c r="O45" s="73"/>
+      <c r="P45" s="73"/>
+      <c r="Q45" s="73"/>
+      <c r="R45" s="73"/>
+      <c r="S45" s="73"/>
+      <c r="T45" s="73"/>
+      <c r="U45" s="73"/>
+      <c r="V45" s="73"/>
+      <c r="W45" s="73"/>
+      <c r="X45" s="73"/>
+      <c r="Y45" s="73"/>
+      <c r="Z45" s="73"/>
+    </row>
+    <row r="46" spans="1:26" s="45" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A46" s="47"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="51"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="42"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="75"/>
+      <c r="F46" s="69"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="8"/>
@@ -2572,13 +2581,13 @@
       <c r="Y46" s="8"/>
       <c r="Z46" s="8"/>
     </row>
-    <row r="47" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A47" s="50"/>
-      <c r="B47" s="55"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="42"/>
+    <row r="47" spans="1:26" s="45" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A47" s="47"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="78"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="69"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="8"/>
@@ -2600,13 +2609,13 @@
       <c r="Y47" s="8"/>
       <c r="Z47" s="8"/>
     </row>
-    <row r="48" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A48" s="50"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="43"/>
+    <row r="48" spans="1:26" s="45" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A48" s="48"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="70"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="8"/>
@@ -2657,10 +2666,10 @@
       <c r="Z49" s="34"/>
     </row>
     <row r="50" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A50" s="50">
+      <c r="A50" s="49">
         <v>5</v>
       </c>
-      <c r="B50" s="55" t="s">
+      <c r="B50" s="53" t="s">
         <v>36</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2669,10 +2678,10 @@
       <c r="E50" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F50" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="G50" s="18"/>
+      <c r="F50" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="G50" s="40"/>
       <c r="H50" s="11"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
@@ -2694,16 +2703,14 @@
       <c r="Z50" s="8"/>
     </row>
     <row r="51" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A51" s="50"/>
-      <c r="B51" s="55"/>
+      <c r="A51" s="49"/>
+      <c r="B51" s="53"/>
       <c r="C51" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E51" s="10"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="61" t="s">
-        <v>110</v>
-      </c>
+      <c r="F51" s="56"/>
+      <c r="G51" s="46"/>
       <c r="H51" s="11"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
@@ -2725,14 +2732,14 @@
       <c r="Z51" s="8"/>
     </row>
     <row r="52" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A52" s="50"/>
-      <c r="B52" s="55"/>
+      <c r="A52" s="49"/>
+      <c r="B52" s="53"/>
       <c r="C52" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E52" s="10"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="18"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="40"/>
       <c r="H52" s="11"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
@@ -2782,23 +2789,23 @@
       <c r="Z53" s="34"/>
     </row>
     <row r="54" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="50">
+      <c r="A54" s="49">
         <v>6</v>
       </c>
-      <c r="B54" s="55" t="s">
+      <c r="B54" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D54" s="51"/>
+      <c r="D54" s="50"/>
       <c r="E54" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F54" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="G54" s="38"/>
+      <c r="F54" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="G54" s="40"/>
       <c r="H54" s="11"/>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
@@ -2820,17 +2827,15 @@
       <c r="Z54" s="8"/>
     </row>
     <row r="55" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A55" s="50"/>
-      <c r="B55" s="55"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="51"/>
+      <c r="A55" s="49"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="50"/>
       <c r="E55" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F55" s="42"/>
-      <c r="G55" s="61" t="s">
-        <v>105</v>
-      </c>
+      <c r="F55" s="56"/>
+      <c r="G55" s="46"/>
       <c r="H55" s="11"/>
       <c r="I55" s="8"/>
       <c r="J55" s="8"/>
@@ -2852,17 +2857,15 @@
       <c r="Z55" s="8"/>
     </row>
     <row r="56" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A56" s="50"/>
-      <c r="B56" s="55"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="51"/>
+      <c r="A56" s="49"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="50"/>
       <c r="E56" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F56" s="43"/>
-      <c r="G56" s="61" t="s">
-        <v>106</v>
-      </c>
+      <c r="F56" s="57"/>
+      <c r="G56" s="46"/>
       <c r="H56" s="11"/>
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
@@ -2911,7 +2914,7 @@
       <c r="Y57" s="34"/>
       <c r="Z57" s="34"/>
     </row>
-    <row r="58" spans="1:26" s="9" customFormat="1" ht="33" customHeight="1">
+    <row r="58" spans="1:26" s="9" customFormat="1" ht="58.5" customHeight="1">
       <c r="A58" s="18">
         <v>7</v>
       </c>
@@ -2923,12 +2926,10 @@
       <c r="E58" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F58" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="G58" s="61" t="s">
-        <v>107</v>
-      </c>
+      <c r="F58" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="G58" s="46"/>
       <c r="H58" s="11"/>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
@@ -2978,10 +2979,10 @@
       <c r="Z59" s="34"/>
     </row>
     <row r="60" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A60" s="44">
+      <c r="A60" s="61">
         <v>8</v>
       </c>
-      <c r="B60" s="47" t="s">
+      <c r="B60" s="62" t="s">
         <v>39</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2991,12 +2992,10 @@
       <c r="E60" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F60" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="G60" s="61" t="s">
-        <v>108</v>
-      </c>
+      <c r="F60" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="G60" s="46"/>
       <c r="H60" s="11"/>
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
@@ -3018,17 +3017,15 @@
       <c r="Z60" s="8"/>
     </row>
     <row r="61" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A61" s="45"/>
-      <c r="B61" s="48"/>
+      <c r="A61" s="47"/>
+      <c r="B61" s="63"/>
       <c r="C61" s="3"/>
       <c r="D61" s="19"/>
       <c r="E61" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F61" s="42"/>
-      <c r="G61" s="61" t="s">
-        <v>109</v>
-      </c>
+      <c r="F61" s="56"/>
+      <c r="G61" s="46"/>
       <c r="H61" s="11"/>
       <c r="I61" s="8"/>
       <c r="J61" s="8"/>
@@ -3050,15 +3047,15 @@
       <c r="Z61" s="8"/>
     </row>
     <row r="62" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A62" s="45"/>
-      <c r="B62" s="48"/>
+      <c r="A62" s="47"/>
+      <c r="B62" s="63"/>
       <c r="C62" s="3"/>
       <c r="D62" s="19"/>
       <c r="E62" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F62" s="42"/>
-      <c r="G62" s="18"/>
+      <c r="F62" s="56"/>
+      <c r="G62" s="40"/>
       <c r="H62" s="11"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -3080,15 +3077,15 @@
       <c r="Z62" s="8"/>
     </row>
     <row r="63" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A63" s="46"/>
-      <c r="B63" s="49"/>
+      <c r="A63" s="48"/>
+      <c r="B63" s="64"/>
       <c r="C63" s="3"/>
       <c r="D63" s="19"/>
       <c r="E63" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F63" s="43"/>
-      <c r="G63" s="18"/>
+      <c r="F63" s="57"/>
+      <c r="G63" s="40"/>
       <c r="H63" s="11"/>
       <c r="I63" s="8"/>
       <c r="J63" s="8"/>
@@ -3150,9 +3147,9 @@
         <v>58</v>
       </c>
       <c r="F65" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="G65" s="18"/>
+        <v>98</v>
+      </c>
+      <c r="G65" s="40"/>
       <c r="H65" s="11"/>
       <c r="I65" s="8"/>
       <c r="J65" s="8"/>
@@ -3174,31 +3171,7 @@
       <c r="Z65" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="G9:G36"/>
-    <mergeCell ref="A9:A27"/>
-    <mergeCell ref="D9:D27"/>
-    <mergeCell ref="F9:F27"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="D44:D48"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="F44:F48"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B27"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
+  <mergeCells count="31">
     <mergeCell ref="F50:F52"/>
     <mergeCell ref="F54:F56"/>
     <mergeCell ref="F60:F63"/>
@@ -3210,6 +3183,26 @@
     <mergeCell ref="A50:A52"/>
     <mergeCell ref="B50:B52"/>
     <mergeCell ref="C55:C56"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B27"/>
+    <mergeCell ref="A9:A27"/>
+    <mergeCell ref="D9:D27"/>
+    <mergeCell ref="F9:F27"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F44:F48"/>
+    <mergeCell ref="F37:F41"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
added admin entity to design document
</commit_message>
<xml_diff>
--- a/Lhub_RTM.xlsx
+++ b/Lhub_RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazmy\Documents\GitHub\Learning-hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project management\Learning-hub project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="7760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20505" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,18 +367,25 @@
 Lhub_SDD_7.1.2.8</t>
   </si>
   <si>
-    <t>Lhub_SDD_4.1.4
+    <t>Lhub_SDD_5.2.4
+Lhub_SDD_7.1.2.6</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.3.10</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.3.11</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_4.1.5
 Lhub_SDD_5.2.3
 Lhub_SDD__6.1.2.2.3
 Lhub_SDD__6.1.2.2.4
 Lhub_SDD_7.1.2.9</t>
   </si>
   <si>
-    <t>Lhub_SDD_5.2.4
-Lhub_SDD_7.1.2.6</t>
-  </si>
-  <si>
-    <t>Lhub_SDD_6.1.3.2.1
+    <t>Lhub_SDD_4.1.4
+Lhub_SDD_6.1.3.2.1
 Lhub_SDD_6.1.6.2.2
 Lhub_SDD_5.2.5
 Lhub_SDD_5.2.6
@@ -387,12 +394,6 @@
 Lhub_SDD_7.1.2.12
 Lhub_SDD_7.1.2.13
 Lhub_SDD_7.1.2.14</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.3.10</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.3.11</t>
   </si>
 </sst>
 </file>
@@ -803,28 +804,61 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -844,39 +878,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1204,21 +1205,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="48.1796875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="35.81640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" style="12" customWidth="1"/>
     <col min="6" max="6" width="38" style="22" customWidth="1"/>
-    <col min="7" max="7" width="37.54296875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="44.54296875" style="12" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="12"/>
+    <col min="7" max="7" width="37.5703125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="4" customFormat="1" ht="30" customHeight="1">
@@ -1231,10 +1232,10 @@
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="73"/>
       <c r="D2" s="23" t="s">
         <v>58</v>
       </c>
@@ -1255,10 +1256,10 @@
       <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="73"/>
       <c r="D3" s="24" t="s">
         <v>63</v>
       </c>
@@ -1279,10 +1280,10 @@
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="75">
+      <c r="B4" s="74">
         <v>43470</v>
       </c>
-      <c r="C4" s="75"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="25"/>
       <c r="E4" s="14">
         <v>43592</v>
@@ -1295,7 +1296,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="7" customFormat="1" ht="25">
+    <row r="5" spans="1:26" s="7" customFormat="1" ht="25.5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1340,22 +1341,22 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" s="9" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A6" s="77">
+      <c r="A6" s="67">
         <v>1</v>
       </c>
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="66" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="78"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="79"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="50"/>
-      <c r="H6" s="79"/>
+      <c r="H6" s="70"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -1376,18 +1377,18 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" spans="1:26" s="9" customFormat="1">
-      <c r="A7" s="77"/>
-      <c r="B7" s="76"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="78"/>
+      <c r="D7" s="68"/>
       <c r="E7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="79"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="50"/>
-      <c r="H7" s="79"/>
+      <c r="H7" s="70"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1436,24 +1437,24 @@
       <c r="Z8" s="34"/>
     </row>
     <row r="9" spans="1:26" s="9" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="77">
+      <c r="A9" s="67">
         <v>2</v>
       </c>
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="66" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="78"/>
+      <c r="D9" s="68"/>
       <c r="E9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="80" t="s">
+      <c r="F9" s="71" t="s">
         <v>100</v>
       </c>
       <c r="G9" s="48"/>
-      <c r="H9" s="77"/>
+      <c r="H9" s="67"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1474,18 +1475,18 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A10" s="77"/>
-      <c r="B10" s="76"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="78"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="81"/>
+      <c r="F10" s="72"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="77"/>
+      <c r="H10" s="67"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1506,16 +1507,16 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="77"/>
-      <c r="B11" s="76"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="78"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="81"/>
+      <c r="F11" s="72"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="8"/>
@@ -1538,16 +1539,16 @@
       <c r="Z11" s="8"/>
     </row>
     <row r="12" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="77"/>
-      <c r="B12" s="76"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="78"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="81"/>
+      <c r="F12" s="72"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="8"/>
@@ -1570,16 +1571,16 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="77"/>
-      <c r="B13" s="76"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="78"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="81"/>
+      <c r="F13" s="72"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="8"/>
@@ -1602,14 +1603,14 @@
       <c r="Z13" s="8"/>
     </row>
     <row r="14" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="77"/>
-      <c r="B14" s="76"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="39"/>
-      <c r="D14" s="78"/>
+      <c r="D14" s="68"/>
       <c r="E14" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="81"/>
+      <c r="F14" s="72"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="8"/>
@@ -1632,14 +1633,14 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="77"/>
-      <c r="B15" s="76"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="39"/>
-      <c r="D15" s="78"/>
+      <c r="D15" s="68"/>
       <c r="E15" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="81"/>
+      <c r="F15" s="72"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="8"/>
@@ -1662,14 +1663,14 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="77"/>
-      <c r="B16" s="76"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="39"/>
-      <c r="D16" s="78"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="81"/>
+      <c r="F16" s="72"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="8"/>
@@ -1692,14 +1693,14 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="77"/>
-      <c r="B17" s="76"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="39"/>
-      <c r="D17" s="78"/>
+      <c r="D17" s="68"/>
       <c r="E17" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="81"/>
+      <c r="F17" s="72"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="8"/>
@@ -1722,14 +1723,14 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="77"/>
-      <c r="B18" s="76"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="39"/>
-      <c r="D18" s="78"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="81"/>
+      <c r="F18" s="72"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="8"/>
@@ -1752,14 +1753,14 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="77"/>
-      <c r="B19" s="76"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="39"/>
-      <c r="D19" s="78"/>
+      <c r="D19" s="68"/>
       <c r="E19" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="81"/>
+      <c r="F19" s="72"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="8"/>
@@ -1782,14 +1783,14 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="77"/>
-      <c r="B20" s="76"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="39"/>
-      <c r="D20" s="78"/>
+      <c r="D20" s="68"/>
       <c r="E20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="81"/>
+      <c r="F20" s="72"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="8"/>
@@ -1812,14 +1813,14 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="77"/>
-      <c r="B21" s="76"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="66"/>
       <c r="C21" s="39"/>
-      <c r="D21" s="78"/>
+      <c r="D21" s="68"/>
       <c r="E21" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="81"/>
+      <c r="F21" s="72"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="8"/>
@@ -1842,14 +1843,14 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="77"/>
-      <c r="B22" s="76"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="39"/>
-      <c r="D22" s="78"/>
+      <c r="D22" s="68"/>
       <c r="E22" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="81"/>
+      <c r="F22" s="72"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="8"/>
@@ -1872,14 +1873,14 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="77"/>
-      <c r="B23" s="76"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="39"/>
-      <c r="D23" s="78"/>
+      <c r="D23" s="68"/>
       <c r="E23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="81"/>
+      <c r="F23" s="72"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="8"/>
@@ -1902,14 +1903,14 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="77"/>
-      <c r="B24" s="76"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="39"/>
-      <c r="D24" s="78"/>
+      <c r="D24" s="68"/>
       <c r="E24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="81"/>
+      <c r="F24" s="72"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="8"/>
@@ -1932,14 +1933,14 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A25" s="77"/>
-      <c r="B25" s="76"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="39"/>
-      <c r="D25" s="78"/>
+      <c r="D25" s="68"/>
       <c r="E25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="81"/>
+      <c r="F25" s="72"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="8"/>
@@ -1962,14 +1963,14 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="77"/>
-      <c r="B26" s="76"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="39"/>
-      <c r="D26" s="78"/>
+      <c r="D26" s="68"/>
       <c r="E26" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="81"/>
+      <c r="F26" s="72"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="8"/>
@@ -1992,14 +1993,14 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="77"/>
-      <c r="B27" s="76"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="66"/>
       <c r="C27" s="39"/>
-      <c r="D27" s="78"/>
+      <c r="D27" s="68"/>
       <c r="E27" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="81"/>
+      <c r="F27" s="72"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="8"/>
@@ -2335,7 +2336,7 @@
       <c r="E38" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="58"/>
+      <c r="F38" s="75"/>
       <c r="G38" s="40"/>
       <c r="H38" s="11"/>
       <c r="I38" s="8"/>
@@ -2366,7 +2367,7 @@
       <c r="E39" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F39" s="58"/>
+      <c r="F39" s="75"/>
       <c r="G39" s="40"/>
       <c r="H39" s="11"/>
       <c r="I39" s="8"/>
@@ -2396,7 +2397,7 @@
       <c r="E40" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F40" s="58"/>
+      <c r="F40" s="75"/>
       <c r="G40" s="40"/>
       <c r="H40" s="11"/>
       <c r="I40" s="8"/>
@@ -2428,7 +2429,7 @@
       <c r="E41" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="F41" s="59"/>
+      <c r="F41" s="76"/>
       <c r="G41" s="40"/>
       <c r="H41" s="11"/>
       <c r="I41" s="8"/>
@@ -2520,7 +2521,7 @@
       <c r="C44" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="66"/>
+      <c r="D44" s="77"/>
       <c r="E44" s="41" t="s">
         <v>85</v>
       </c>
@@ -2556,11 +2557,11 @@
       <c r="C45" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="67"/>
+      <c r="D45" s="78"/>
       <c r="E45" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="F45" s="58"/>
+      <c r="F45" s="75"/>
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
       <c r="I45" s="54"/>
@@ -2588,9 +2589,9 @@
       <c r="C46" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="67"/>
-      <c r="E46" s="71"/>
-      <c r="F46" s="58"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="75"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="8"/>
@@ -2615,10 +2616,10 @@
     <row r="47" spans="1:26" s="45" customFormat="1" ht="18.75" customHeight="1">
       <c r="A47" s="61"/>
       <c r="B47" s="64"/>
-      <c r="C47" s="69"/>
-      <c r="D47" s="67"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="58"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="83"/>
+      <c r="F47" s="75"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="8"/>
@@ -2643,10 +2644,10 @@
     <row r="48" spans="1:26" s="45" customFormat="1" ht="19.5" customHeight="1">
       <c r="A48" s="62"/>
       <c r="B48" s="65"/>
-      <c r="C48" s="70"/>
-      <c r="D48" s="68"/>
-      <c r="E48" s="73"/>
-      <c r="F48" s="59"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="79"/>
+      <c r="E48" s="84"/>
+      <c r="F48" s="76"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="8"/>
@@ -2697,10 +2698,10 @@
       <c r="Z49" s="34"/>
     </row>
     <row r="50" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A50" s="77">
+      <c r="A50" s="67">
         <v>5</v>
       </c>
-      <c r="B50" s="76" t="s">
+      <c r="B50" s="66" t="s">
         <v>36</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2734,13 +2735,13 @@
       <c r="Z50" s="8"/>
     </row>
     <row r="51" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A51" s="77"/>
-      <c r="B51" s="76"/>
+      <c r="A51" s="67"/>
+      <c r="B51" s="66"/>
       <c r="C51" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E51" s="10"/>
-      <c r="F51" s="82"/>
+      <c r="F51" s="58"/>
       <c r="G51" s="46"/>
       <c r="H51" s="11"/>
       <c r="I51" s="8"/>
@@ -2763,13 +2764,13 @@
       <c r="Z51" s="8"/>
     </row>
     <row r="52" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A52" s="77"/>
-      <c r="B52" s="76"/>
+      <c r="A52" s="67"/>
+      <c r="B52" s="66"/>
       <c r="C52" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E52" s="10"/>
-      <c r="F52" s="83"/>
+      <c r="F52" s="59"/>
       <c r="G52" s="40"/>
       <c r="H52" s="11"/>
       <c r="I52" s="8"/>
@@ -2820,21 +2821,21 @@
       <c r="Z53" s="34"/>
     </row>
     <row r="54" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="77">
+      <c r="A54" s="67">
         <v>6</v>
       </c>
-      <c r="B54" s="76" t="s">
+      <c r="B54" s="66" t="s">
         <v>37</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D54" s="78"/>
+      <c r="D54" s="68"/>
       <c r="E54" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F54" s="57" t="s">
         <v>108</v>
-      </c>
-      <c r="F54" s="57" t="s">
-        <v>105</v>
       </c>
       <c r="G54" s="40"/>
       <c r="H54" s="11"/>
@@ -2858,14 +2859,14 @@
       <c r="Z54" s="8"/>
     </row>
     <row r="55" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A55" s="77"/>
-      <c r="B55" s="76"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="78"/>
+      <c r="A55" s="67"/>
+      <c r="B55" s="66"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="68"/>
       <c r="E55" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F55" s="82"/>
+        <v>107</v>
+      </c>
+      <c r="F55" s="58"/>
       <c r="G55" s="46"/>
       <c r="H55" s="11"/>
       <c r="I55" s="8"/>
@@ -2888,12 +2889,12 @@
       <c r="Z55" s="8"/>
     </row>
     <row r="56" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A56" s="77"/>
-      <c r="B56" s="76"/>
-      <c r="C56" s="84"/>
-      <c r="D56" s="78"/>
+      <c r="A56" s="67"/>
+      <c r="B56" s="66"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="68"/>
       <c r="E56" s="10"/>
-      <c r="F56" s="83"/>
+      <c r="F56" s="59"/>
       <c r="G56" s="46"/>
       <c r="H56" s="11"/>
       <c r="I56" s="8"/>
@@ -2943,7 +2944,7 @@
       <c r="Y57" s="34"/>
       <c r="Z57" s="34"/>
     </row>
-    <row r="58" spans="1:26" s="9" customFormat="1" ht="67.75" customHeight="1">
+    <row r="58" spans="1:26" s="9" customFormat="1" ht="67.7" customHeight="1">
       <c r="A58" s="18">
         <v>7</v>
       </c>
@@ -3024,7 +3025,7 @@
         <v>55</v>
       </c>
       <c r="F60" s="57" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G60" s="46"/>
       <c r="H60" s="11"/>
@@ -3057,7 +3058,7 @@
       <c r="E61" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F61" s="82"/>
+      <c r="F61" s="58"/>
       <c r="G61" s="46"/>
       <c r="H61" s="11"/>
       <c r="I61" s="8"/>
@@ -3087,7 +3088,7 @@
       <c r="E62" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F62" s="82"/>
+      <c r="F62" s="58"/>
       <c r="G62" s="40"/>
       <c r="H62" s="11"/>
       <c r="I62" s="8"/>
@@ -3117,7 +3118,7 @@
       <c r="E63" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F63" s="83"/>
+      <c r="F63" s="59"/>
       <c r="G63" s="40"/>
       <c r="H63" s="11"/>
       <c r="I63" s="8"/>
@@ -3180,7 +3181,7 @@
         <v>57</v>
       </c>
       <c r="F65" s="56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G65" s="40"/>
       <c r="H65" s="11"/>
@@ -3205,6 +3206,26 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="F44:F48"/>
+    <mergeCell ref="F37:F41"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B27"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A9:A27"/>
+    <mergeCell ref="D9:D27"/>
+    <mergeCell ref="F9:F27"/>
     <mergeCell ref="F50:F52"/>
     <mergeCell ref="F54:F56"/>
     <mergeCell ref="F60:F63"/>
@@ -3216,26 +3237,6 @@
     <mergeCell ref="A50:A52"/>
     <mergeCell ref="B50:B52"/>
     <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A9:A27"/>
-    <mergeCell ref="D9:D27"/>
-    <mergeCell ref="F9:F27"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B27"/>
-    <mergeCell ref="F44:F48"/>
-    <mergeCell ref="F37:F41"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="D44:D48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="E46:E48"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
update rtm home page
</commit_message>
<xml_diff>
--- a/Lhub_RTM.xlsx
+++ b/Lhub_RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI subjects\software project management\project 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA_project\Edit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="7404"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="23004" windowHeight="7404"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="134">
   <si>
     <t>Project Name:</t>
   </si>
@@ -440,6 +440,44 @@
   <si>
     <t>lhub_login_8</t>
   </si>
+  <si>
+    <t>HM_17</t>
+  </si>
+  <si>
+    <t>HM_11</t>
+  </si>
+  <si>
+    <t>HM_19
+HM_20</t>
+  </si>
+  <si>
+    <t>HM_21
+HM_22
+HM_23</t>
+  </si>
+  <si>
+    <t>HM_24
+HM_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM_26
+HM_27
+HM_03
+</t>
+  </si>
+  <si>
+    <t>HM_28
+HM_29</t>
+  </si>
+  <si>
+    <t>HM_04</t>
+  </si>
+  <si>
+    <t>HM_13
+HM_14
+HM_15
+HM_16</t>
+  </si>
 </sst>
 </file>
 
@@ -448,7 +486,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,8 +600,15 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +648,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,7 +761,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -877,6 +928,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -962,17 +1016,26 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1301,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.296875" defaultRowHeight="17.399999999999999"/>
@@ -1322,21 +1385,21 @@
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
       <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="82"/>
+      <c r="C2" s="83"/>
       <c r="D2" s="59" t="s">
         <v>51</v>
       </c>
@@ -1357,10 +1420,10 @@
       <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="82"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="13">
         <v>1</v>
       </c>
@@ -1381,10 +1444,10 @@
       <c r="A4" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="83">
+      <c r="B4" s="84">
         <v>43470</v>
       </c>
-      <c r="C4" s="83"/>
+      <c r="C4" s="84"/>
       <c r="D4" s="13">
         <v>1.1000000000000001</v>
       </c>
@@ -1403,8 +1466,8 @@
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A5" s="42"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="64"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
       <c r="D5" s="13">
         <v>1.2</v>
       </c>
@@ -1466,10 +1529,10 @@
       </c>
     </row>
     <row r="8" spans="1:26" s="4" customFormat="1" ht="37.950000000000003" customHeight="1">
-      <c r="A8" s="85">
+      <c r="A8" s="86">
         <v>1</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="85" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -1479,9 +1542,9 @@
       <c r="E8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="86"/>
+      <c r="F8" s="87"/>
       <c r="G8" s="36"/>
-      <c r="H8" s="86"/>
+      <c r="H8" s="87"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1502,8 +1565,8 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="85"/>
-      <c r="B9" s="84"/>
+      <c r="A9" s="86"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
@@ -1511,9 +1574,9 @@
       <c r="E9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="86"/>
+      <c r="F9" s="87"/>
       <c r="G9" s="36"/>
-      <c r="H9" s="86"/>
+      <c r="H9" s="87"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1562,10 +1625,10 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A11" s="85">
+      <c r="A11" s="86">
         <v>2</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="85" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="21" t="s">
@@ -1577,13 +1640,13 @@
       <c r="E11" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="87" t="s">
+      <c r="F11" s="88" t="s">
         <v>87</v>
       </c>
       <c r="G11" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="H11" s="85"/>
+      <c r="H11" s="86"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1604,8 +1667,8 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="85"/>
-      <c r="B12" s="84"/>
+      <c r="A12" s="86"/>
+      <c r="B12" s="85"/>
       <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
@@ -1615,8 +1678,8 @@
       <c r="E12" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="88"/>
-      <c r="H12" s="85"/>
+      <c r="F12" s="89"/>
+      <c r="H12" s="86"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1637,8 +1700,8 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="85"/>
-      <c r="B13" s="84"/>
+      <c r="A13" s="86"/>
+      <c r="B13" s="85"/>
       <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
@@ -1648,7 +1711,7 @@
       <c r="E13" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="88"/>
+      <c r="F13" s="89"/>
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="3"/>
@@ -1671,8 +1734,8 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="85"/>
-      <c r="B14" s="84"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="85"/>
       <c r="C14" s="21" t="s">
         <v>83</v>
       </c>
@@ -1682,7 +1745,7 @@
       <c r="E14" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="88"/>
+      <c r="F14" s="89"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="3"/>
@@ -1705,8 +1768,8 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="85"/>
-      <c r="B15" s="84"/>
+      <c r="A15" s="86"/>
+      <c r="B15" s="85"/>
       <c r="C15" s="21" t="s">
         <v>80</v>
       </c>
@@ -1716,7 +1779,7 @@
       <c r="E15" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="88"/>
+      <c r="F15" s="89"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="3"/>
@@ -1739,8 +1802,8 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="85"/>
-      <c r="B16" s="84"/>
+      <c r="A16" s="86"/>
+      <c r="B16" s="85"/>
       <c r="C16" s="23"/>
       <c r="D16" s="60" t="s">
         <v>117</v>
@@ -1748,7 +1811,7 @@
       <c r="E16" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="88"/>
+      <c r="F16" s="89"/>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="3"/>
@@ -1771,8 +1834,8 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="85"/>
-      <c r="B17" s="84"/>
+      <c r="A17" s="86"/>
+      <c r="B17" s="85"/>
       <c r="C17" s="23"/>
       <c r="D17" s="60" t="s">
         <v>122</v>
@@ -1780,7 +1843,7 @@
       <c r="E17" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="88"/>
+      <c r="F17" s="89"/>
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="3"/>
@@ -1803,8 +1866,8 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="85"/>
-      <c r="B18" s="84"/>
+      <c r="A18" s="86"/>
+      <c r="B18" s="85"/>
       <c r="C18" s="23"/>
       <c r="D18" s="60" t="s">
         <v>123</v>
@@ -1812,7 +1875,7 @@
       <c r="E18" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="88"/>
+      <c r="F18" s="89"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="3"/>
@@ -1835,8 +1898,8 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="85"/>
-      <c r="B19" s="84"/>
+      <c r="A19" s="86"/>
+      <c r="B19" s="85"/>
       <c r="C19" s="23"/>
       <c r="D19" s="60" t="s">
         <v>117</v>
@@ -1844,7 +1907,7 @@
       <c r="E19" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="88"/>
+      <c r="F19" s="89"/>
       <c r="G19" s="37"/>
       <c r="H19" s="37"/>
       <c r="I19" s="3"/>
@@ -1867,8 +1930,8 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="85"/>
-      <c r="B20" s="84"/>
+      <c r="A20" s="86"/>
+      <c r="B20" s="85"/>
       <c r="C20" s="23"/>
       <c r="D20" s="60" t="s">
         <v>124</v>
@@ -1876,7 +1939,7 @@
       <c r="E20" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="88"/>
+      <c r="F20" s="89"/>
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
       <c r="I20" s="3"/>
@@ -1899,12 +1962,12 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="85"/>
-      <c r="B21" s="84"/>
+      <c r="A21" s="86"/>
+      <c r="B21" s="85"/>
       <c r="C21" s="23"/>
       <c r="D21" s="60"/>
       <c r="E21" s="92"/>
-      <c r="F21" s="88"/>
+      <c r="F21" s="89"/>
       <c r="G21" s="52" t="s">
         <v>115</v>
       </c>
@@ -1929,12 +1992,12 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="85"/>
-      <c r="B22" s="84"/>
+      <c r="A22" s="86"/>
+      <c r="B22" s="85"/>
       <c r="C22" s="23"/>
       <c r="D22" s="60"/>
       <c r="E22" s="93"/>
-      <c r="F22" s="88"/>
+      <c r="F22" s="89"/>
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
       <c r="I22" s="3"/>
@@ -1957,12 +2020,12 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="85"/>
-      <c r="B23" s="84"/>
+      <c r="A23" s="86"/>
+      <c r="B23" s="85"/>
       <c r="C23" s="23"/>
       <c r="D23" s="60"/>
       <c r="E23" s="93"/>
-      <c r="F23" s="88"/>
+      <c r="F23" s="89"/>
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
       <c r="I23" s="3"/>
@@ -1985,12 +2048,12 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="85"/>
-      <c r="B24" s="84"/>
+      <c r="A24" s="86"/>
+      <c r="B24" s="85"/>
       <c r="C24" s="23"/>
       <c r="D24" s="60"/>
       <c r="E24" s="94"/>
-      <c r="F24" s="88"/>
+      <c r="F24" s="89"/>
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
       <c r="I24" s="3"/>
@@ -2013,14 +2076,14 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
-      <c r="A25" s="85"/>
-      <c r="B25" s="84"/>
+      <c r="A25" s="86"/>
+      <c r="B25" s="85"/>
       <c r="C25" s="23"/>
       <c r="D25" s="60"/>
       <c r="E25" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="88"/>
+      <c r="F25" s="89"/>
       <c r="G25" s="56" t="s">
         <v>112</v>
       </c>
@@ -2045,14 +2108,14 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="85"/>
-      <c r="B26" s="84"/>
+      <c r="A26" s="86"/>
+      <c r="B26" s="85"/>
       <c r="C26" s="23"/>
       <c r="D26" s="60"/>
       <c r="E26" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="88"/>
+      <c r="F26" s="89"/>
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
       <c r="I26" s="3"/>
@@ -2075,14 +2138,14 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="85"/>
-      <c r="B27" s="84"/>
+      <c r="A27" s="86"/>
+      <c r="B27" s="85"/>
       <c r="C27" s="23"/>
       <c r="D27" s="60"/>
       <c r="E27" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="88"/>
+      <c r="F27" s="89"/>
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
       <c r="I27" s="3"/>
@@ -2105,14 +2168,14 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="85"/>
-      <c r="B28" s="84"/>
+      <c r="A28" s="86"/>
+      <c r="B28" s="85"/>
       <c r="C28" s="23"/>
       <c r="D28" s="60"/>
       <c r="E28" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="88"/>
+      <c r="F28" s="89"/>
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
       <c r="I28" s="3"/>
@@ -2135,14 +2198,14 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="85"/>
-      <c r="B29" s="84"/>
+      <c r="A29" s="86"/>
+      <c r="B29" s="85"/>
       <c r="C29" s="23"/>
       <c r="D29" s="60"/>
       <c r="E29" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="88"/>
+      <c r="F29" s="89"/>
       <c r="G29" s="37"/>
       <c r="H29" s="37"/>
       <c r="I29" s="3"/>
@@ -2472,11 +2535,13 @@
       <c r="C40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="27"/>
+      <c r="D40" s="96" t="s">
+        <v>125</v>
+      </c>
       <c r="E40" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="65" t="s">
+      <c r="F40" s="66" t="s">
         <v>88</v>
       </c>
       <c r="G40" s="12"/>
@@ -2506,11 +2571,13 @@
       <c r="C41" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="27"/>
+      <c r="D41" s="96" t="s">
+        <v>126</v>
+      </c>
       <c r="E41" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="66"/>
+      <c r="F41" s="67"/>
       <c r="G41" s="12"/>
       <c r="H41" s="37"/>
       <c r="I41" s="3"/>
@@ -2532,17 +2599,19 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
+    <row r="42" spans="1:26" s="8" customFormat="1" ht="51.6" customHeight="1">
       <c r="A42" s="12"/>
       <c r="B42" s="19"/>
       <c r="C42" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="27"/>
+      <c r="D42" s="97" t="s">
+        <v>127</v>
+      </c>
       <c r="E42" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="66"/>
+      <c r="F42" s="67"/>
       <c r="G42" s="12"/>
       <c r="H42" s="37"/>
       <c r="I42" s="3"/>
@@ -2564,15 +2633,17 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
+    <row r="43" spans="1:26" s="8" customFormat="1" ht="59.4" customHeight="1">
       <c r="A43" s="12"/>
       <c r="B43" s="19"/>
       <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
+      <c r="D43" s="97" t="s">
+        <v>127</v>
+      </c>
       <c r="E43" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="F43" s="66"/>
+      <c r="F43" s="67"/>
       <c r="G43" s="12"/>
       <c r="H43" s="37"/>
       <c r="I43" s="3"/>
@@ -2600,11 +2671,11 @@
       <c r="C44" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="21"/>
+      <c r="D44" s="51"/>
       <c r="E44" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="67"/>
+      <c r="F44" s="68"/>
       <c r="G44" s="12"/>
       <c r="H44" s="37"/>
       <c r="I44" s="3"/>
@@ -2632,7 +2703,7 @@
       <c r="C45" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="21"/>
+      <c r="D45" s="51"/>
       <c r="E45" s="30"/>
       <c r="F45" s="33" t="s">
         <v>78</v>
@@ -2687,20 +2758,22 @@
       <c r="Z46" s="6"/>
     </row>
     <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="68">
+      <c r="A47" s="69">
         <v>4</v>
       </c>
-      <c r="B47" s="71" t="s">
+      <c r="B47" s="72" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="74"/>
+      <c r="D47" s="75" t="s">
+        <v>128</v>
+      </c>
       <c r="E47" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="65" t="s">
+      <c r="F47" s="66" t="s">
         <v>89</v>
       </c>
       <c r="G47" s="37" t="s">
@@ -2727,16 +2800,16 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A48" s="69"/>
-      <c r="B48" s="72"/>
+      <c r="A48" s="70"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="75"/>
+      <c r="D48" s="76"/>
       <c r="E48" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="F48" s="66"/>
+      <c r="F48" s="67"/>
       <c r="G48" s="38"/>
       <c r="H48" s="38"/>
       <c r="I48" s="9"/>
@@ -2759,14 +2832,14 @@
       <c r="Z48" s="9"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="69"/>
-      <c r="B49" s="72"/>
+      <c r="A49" s="70"/>
+      <c r="B49" s="73"/>
       <c r="C49" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="75"/>
-      <c r="E49" s="79"/>
-      <c r="F49" s="66"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="80"/>
+      <c r="F49" s="67"/>
       <c r="G49" s="37"/>
       <c r="H49" s="37"/>
       <c r="I49" s="3"/>
@@ -2789,12 +2862,12 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="69"/>
-      <c r="B50" s="72"/>
-      <c r="C50" s="77"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="80"/>
-      <c r="F50" s="66"/>
+      <c r="A50" s="70"/>
+      <c r="B50" s="73"/>
+      <c r="C50" s="78"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="67"/>
       <c r="G50" s="37"/>
       <c r="H50" s="37"/>
       <c r="I50" s="3"/>
@@ -2817,12 +2890,12 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A51" s="70"/>
-      <c r="B51" s="73"/>
-      <c r="C51" s="78"/>
-      <c r="D51" s="76"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="67"/>
+      <c r="A51" s="71"/>
+      <c r="B51" s="74"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="77"/>
+      <c r="E51" s="82"/>
+      <c r="F51" s="68"/>
       <c r="G51" s="37"/>
       <c r="H51" s="37"/>
       <c r="I51" s="3"/>
@@ -2872,21 +2945,23 @@
       <c r="Y52" s="6"/>
       <c r="Z52" s="6"/>
     </row>
-    <row r="53" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A53" s="85">
+    <row r="53" spans="1:26" s="4" customFormat="1" ht="46.8" customHeight="1">
+      <c r="A53" s="86">
         <v>5</v>
       </c>
-      <c r="B53" s="84" t="s">
+      <c r="B53" s="85" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="27"/>
+      <c r="D53" s="97" t="s">
+        <v>129</v>
+      </c>
       <c r="E53" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F53" s="65" t="s">
+      <c r="F53" s="66" t="s">
         <v>90</v>
       </c>
       <c r="G53" s="12"/>
@@ -2911,14 +2986,14 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="85"/>
-      <c r="B54" s="84"/>
+      <c r="A54" s="86"/>
+      <c r="B54" s="85"/>
       <c r="C54" s="21" t="s">
         <v>25</v>
       </c>
       <c r="D54" s="27"/>
       <c r="E54" s="29"/>
-      <c r="F54" s="89"/>
+      <c r="F54" s="90"/>
       <c r="G54" s="40"/>
       <c r="H54" s="37"/>
       <c r="I54" s="3"/>
@@ -2941,14 +3016,14 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A55" s="85"/>
-      <c r="B55" s="84"/>
+      <c r="A55" s="86"/>
+      <c r="B55" s="85"/>
       <c r="C55" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D55" s="27"/>
       <c r="E55" s="29"/>
-      <c r="F55" s="90"/>
+      <c r="F55" s="91"/>
       <c r="G55" s="12"/>
       <c r="H55" s="37"/>
       <c r="I55" s="3"/>
@@ -2999,18 +3074,20 @@
       <c r="Z56" s="6"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A57" s="85">
+      <c r="A57" s="86">
         <v>6</v>
       </c>
-      <c r="B57" s="84" t="s">
+      <c r="B57" s="85" t="s">
         <v>35</v>
       </c>
       <c r="C57" s="23"/>
-      <c r="D57" s="91"/>
+      <c r="D57" s="95" t="s">
+        <v>130</v>
+      </c>
       <c r="E57" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F57" s="65" t="s">
+      <c r="F57" s="66" t="s">
         <v>92</v>
       </c>
       <c r="G57" s="12"/>
@@ -3035,13 +3112,13 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A58" s="85"/>
-      <c r="B58" s="84"/>
-      <c r="D58" s="91"/>
+      <c r="A58" s="86"/>
+      <c r="B58" s="85"/>
+      <c r="D58" s="95"/>
       <c r="E58" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="F58" s="89"/>
+      <c r="F58" s="90"/>
       <c r="G58" s="40"/>
       <c r="H58" s="37"/>
       <c r="I58" s="3"/>
@@ -3064,16 +3141,16 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A59" s="85"/>
-      <c r="B59" s="84"/>
+      <c r="A59" s="86"/>
+      <c r="B59" s="85"/>
       <c r="C59" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="74"/>
+      <c r="D59" s="75"/>
       <c r="E59" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="F59" s="90"/>
+      <c r="F59" s="91"/>
       <c r="G59" s="40"/>
       <c r="H59" s="37"/>
       <c r="I59" s="3"/>
@@ -3095,11 +3172,13 @@
       <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
     </row>
-    <row r="60" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
+    <row r="60" spans="1:26" s="8" customFormat="1" ht="47.4" customHeight="1">
       <c r="A60" s="48"/>
       <c r="B60" s="47"/>
       <c r="C60" s="51"/>
-      <c r="D60" s="28"/>
+      <c r="D60" s="28" t="s">
+        <v>131</v>
+      </c>
       <c r="E60" s="49" t="s">
         <v>96</v>
       </c>
@@ -3125,11 +3204,13 @@
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
+    <row r="61" spans="1:26" s="8" customFormat="1" ht="69.599999999999994" customHeight="1">
       <c r="A61" s="48"/>
       <c r="B61" s="47"/>
       <c r="C61" s="51"/>
-      <c r="D61" s="28"/>
+      <c r="D61" s="28" t="s">
+        <v>132</v>
+      </c>
       <c r="E61" s="49" t="s">
         <v>109</v>
       </c>
@@ -3193,7 +3274,7 @@
       <c r="C63" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D63" s="26"/>
+      <c r="D63" s="61"/>
       <c r="E63" s="32" t="s">
         <v>97</v>
       </c>
@@ -3252,20 +3333,20 @@
       <c r="Z64" s="6"/>
     </row>
     <row r="65" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A65" s="68">
+      <c r="A65" s="69">
         <v>8</v>
       </c>
-      <c r="B65" s="71" t="s">
+      <c r="B65" s="72" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D65" s="26"/>
+      <c r="D65" s="61"/>
       <c r="E65" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="65" t="s">
+      <c r="F65" s="66" t="s">
         <v>94</v>
       </c>
       <c r="G65" s="40" t="s">
@@ -3292,16 +3373,16 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="69"/>
-      <c r="B66" s="72"/>
+      <c r="A66" s="70"/>
+      <c r="B66" s="73"/>
       <c r="C66" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D66" s="26"/>
+      <c r="D66" s="61"/>
       <c r="E66" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="89"/>
+      <c r="F66" s="90"/>
       <c r="G66" s="40"/>
       <c r="H66" s="37"/>
       <c r="I66" s="3"/>
@@ -3324,16 +3405,16 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="69"/>
-      <c r="B67" s="72"/>
+      <c r="A67" s="70"/>
+      <c r="B67" s="73"/>
       <c r="C67" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D67" s="26"/>
+      <c r="D67" s="61"/>
       <c r="E67" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F67" s="89"/>
+      <c r="F67" s="90"/>
       <c r="G67" s="12"/>
       <c r="H67" s="37"/>
       <c r="I67" s="3"/>
@@ -3356,12 +3437,12 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="70"/>
-      <c r="B68" s="73"/>
+      <c r="A68" s="71"/>
+      <c r="B68" s="74"/>
       <c r="C68" s="21"/>
-      <c r="D68" s="26"/>
+      <c r="D68" s="61"/>
       <c r="E68" s="20"/>
-      <c r="F68" s="90"/>
+      <c r="F68" s="91"/>
       <c r="G68" s="12"/>
       <c r="H68" s="37"/>
       <c r="I68" s="3"/>
@@ -3411,7 +3492,7 @@
       <c r="Y69" s="6"/>
       <c r="Z69" s="6"/>
     </row>
-    <row r="70" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+    <row r="70" spans="1:26" s="4" customFormat="1" ht="91.2" customHeight="1">
       <c r="A70" s="12">
         <v>9</v>
       </c>
@@ -3419,7 +3500,9 @@
         <v>50</v>
       </c>
       <c r="C70" s="21"/>
-      <c r="D70" s="26"/>
+      <c r="D70" s="98" t="s">
+        <v>133</v>
+      </c>
       <c r="E70" s="30" t="s">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
add the test cases IDs of Farah to RTM
note: farah has a problem that she could not access master branch , so she asked me to do this on behalf of her
</commit_message>
<xml_diff>
--- a/Lhub_RTM.xlsx
+++ b/Lhub_RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA_project\Edit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI subjects\software project management\project 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="23004" windowHeight="7404"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="7404"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="138">
   <si>
     <t>Project Name:</t>
   </si>
@@ -477,6 +477,23 @@
 HM_14
 HM_15
 HM_16</t>
+  </si>
+  <si>
+    <t>AM_1,
+AM_2,
+AM_3 ,AM_5 ,AM_6,AM_7</t>
+  </si>
+  <si>
+    <t>AM_1,
+AM_2,
+AM_3 ,AM_5,AM_6,
+AM_7</t>
+  </si>
+  <si>
+    <t>AM_4 ,AM_8</t>
+  </si>
+  <si>
+    <t>AM_9</t>
   </si>
 </sst>
 </file>
@@ -761,7 +778,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -932,6 +949,72 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -944,34 +1027,10 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -995,46 +1054,10 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1364,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="C56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.296875" defaultRowHeight="17.399999999999999"/>
@@ -1385,21 +1408,21 @@
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="84" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
       <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="83"/>
+      <c r="C2" s="97"/>
       <c r="D2" s="59" t="s">
         <v>51</v>
       </c>
@@ -1420,10 +1443,10 @@
       <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="83"/>
+      <c r="C3" s="97"/>
       <c r="D3" s="13">
         <v>1</v>
       </c>
@@ -1444,10 +1467,10 @@
       <c r="A4" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="84">
+      <c r="B4" s="98">
         <v>43470</v>
       </c>
-      <c r="C4" s="84"/>
+      <c r="C4" s="98"/>
       <c r="D4" s="13">
         <v>1.1000000000000001</v>
       </c>
@@ -1466,8 +1489,8 @@
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A5" s="42"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="87"/>
       <c r="D5" s="13">
         <v>1.2</v>
       </c>
@@ -1529,10 +1552,10 @@
       </c>
     </row>
     <row r="8" spans="1:26" s="4" customFormat="1" ht="37.950000000000003" customHeight="1">
-      <c r="A8" s="86">
+      <c r="A8" s="75">
         <v>1</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="74" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -1542,9 +1565,9 @@
       <c r="E8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="87"/>
+      <c r="F8" s="78"/>
       <c r="G8" s="36"/>
-      <c r="H8" s="87"/>
+      <c r="H8" s="78"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1565,8 +1588,8 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="86"/>
-      <c r="B9" s="85"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
@@ -1574,9 +1597,9 @@
       <c r="E9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="87"/>
+      <c r="F9" s="78"/>
       <c r="G9" s="36"/>
-      <c r="H9" s="87"/>
+      <c r="H9" s="78"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1625,10 +1648,10 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A11" s="86">
+      <c r="A11" s="75">
         <v>2</v>
       </c>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="74" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="21" t="s">
@@ -1640,13 +1663,13 @@
       <c r="E11" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="79" t="s">
         <v>87</v>
       </c>
       <c r="G11" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="H11" s="86"/>
+      <c r="H11" s="75"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1667,8 +1690,8 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="86"/>
-      <c r="B12" s="85"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
@@ -1678,8 +1701,8 @@
       <c r="E12" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="89"/>
-      <c r="H12" s="86"/>
+      <c r="F12" s="80"/>
+      <c r="H12" s="75"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1700,8 +1723,8 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="86"/>
-      <c r="B13" s="85"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
@@ -1711,7 +1734,7 @@
       <c r="E13" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="89"/>
+      <c r="F13" s="80"/>
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="3"/>
@@ -1734,8 +1757,8 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="86"/>
-      <c r="B14" s="85"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="21" t="s">
         <v>83</v>
       </c>
@@ -1745,7 +1768,7 @@
       <c r="E14" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="89"/>
+      <c r="F14" s="80"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="3"/>
@@ -1768,8 +1791,8 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="86"/>
-      <c r="B15" s="85"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="21" t="s">
         <v>80</v>
       </c>
@@ -1779,7 +1802,7 @@
       <c r="E15" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="89"/>
+      <c r="F15" s="80"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="3"/>
@@ -1802,8 +1825,8 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="86"/>
-      <c r="B16" s="85"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="74"/>
       <c r="C16" s="23"/>
       <c r="D16" s="60" t="s">
         <v>117</v>
@@ -1811,7 +1834,7 @@
       <c r="E16" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="89"/>
+      <c r="F16" s="80"/>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="3"/>
@@ -1834,8 +1857,8 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="86"/>
-      <c r="B17" s="85"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="23"/>
       <c r="D17" s="60" t="s">
         <v>122</v>
@@ -1843,7 +1866,7 @@
       <c r="E17" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="89"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="3"/>
@@ -1866,8 +1889,8 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="86"/>
-      <c r="B18" s="85"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="23"/>
       <c r="D18" s="60" t="s">
         <v>123</v>
@@ -1875,7 +1898,7 @@
       <c r="E18" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="89"/>
+      <c r="F18" s="80"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="3"/>
@@ -1898,8 +1921,8 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="86"/>
-      <c r="B19" s="85"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="23"/>
       <c r="D19" s="60" t="s">
         <v>117</v>
@@ -1907,7 +1930,7 @@
       <c r="E19" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="89"/>
+      <c r="F19" s="80"/>
       <c r="G19" s="37"/>
       <c r="H19" s="37"/>
       <c r="I19" s="3"/>
@@ -1930,8 +1953,8 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="86"/>
-      <c r="B20" s="85"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="23"/>
       <c r="D20" s="60" t="s">
         <v>124</v>
@@ -1939,7 +1962,7 @@
       <c r="E20" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="89"/>
+      <c r="F20" s="80"/>
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
       <c r="I20" s="3"/>
@@ -1962,12 +1985,12 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="86"/>
-      <c r="B21" s="85"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="23"/>
       <c r="D21" s="60"/>
-      <c r="E21" s="92"/>
-      <c r="F21" s="89"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="80"/>
       <c r="G21" s="52" t="s">
         <v>115</v>
       </c>
@@ -1992,12 +2015,12 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="86"/>
-      <c r="B22" s="85"/>
+      <c r="A22" s="75"/>
+      <c r="B22" s="74"/>
       <c r="C22" s="23"/>
       <c r="D22" s="60"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="89"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="80"/>
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
       <c r="I22" s="3"/>
@@ -2020,12 +2043,12 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="86"/>
-      <c r="B23" s="85"/>
+      <c r="A23" s="75"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="23"/>
       <c r="D23" s="60"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="89"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="80"/>
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
       <c r="I23" s="3"/>
@@ -2048,12 +2071,12 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="86"/>
-      <c r="B24" s="85"/>
+      <c r="A24" s="75"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="23"/>
       <c r="D24" s="60"/>
-      <c r="E24" s="94"/>
-      <c r="F24" s="89"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="80"/>
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
       <c r="I24" s="3"/>
@@ -2076,14 +2099,14 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
-      <c r="A25" s="86"/>
-      <c r="B25" s="85"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="74"/>
       <c r="C25" s="23"/>
       <c r="D25" s="60"/>
       <c r="E25" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="89"/>
+      <c r="F25" s="80"/>
       <c r="G25" s="56" t="s">
         <v>112</v>
       </c>
@@ -2108,14 +2131,14 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="86"/>
-      <c r="B26" s="85"/>
+      <c r="A26" s="75"/>
+      <c r="B26" s="74"/>
       <c r="C26" s="23"/>
       <c r="D26" s="60"/>
       <c r="E26" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="89"/>
+      <c r="F26" s="80"/>
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
       <c r="I26" s="3"/>
@@ -2138,14 +2161,14 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="86"/>
-      <c r="B27" s="85"/>
+      <c r="A27" s="75"/>
+      <c r="B27" s="74"/>
       <c r="C27" s="23"/>
       <c r="D27" s="60"/>
       <c r="E27" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="89"/>
+      <c r="F27" s="80"/>
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
       <c r="I27" s="3"/>
@@ -2168,14 +2191,14 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="86"/>
-      <c r="B28" s="85"/>
+      <c r="A28" s="75"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="23"/>
       <c r="D28" s="60"/>
       <c r="E28" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="89"/>
+      <c r="F28" s="80"/>
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
       <c r="I28" s="3"/>
@@ -2198,14 +2221,14 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="86"/>
-      <c r="B29" s="85"/>
+      <c r="A29" s="75"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="23"/>
       <c r="D29" s="60"/>
       <c r="E29" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="89"/>
+      <c r="F29" s="80"/>
       <c r="G29" s="37"/>
       <c r="H29" s="37"/>
       <c r="I29" s="3"/>
@@ -2535,13 +2558,13 @@
       <c r="C40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="96" t="s">
+      <c r="D40" s="62" t="s">
         <v>125</v>
       </c>
       <c r="E40" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="66" t="s">
+      <c r="F40" s="65" t="s">
         <v>88</v>
       </c>
       <c r="G40" s="12"/>
@@ -2571,13 +2594,13 @@
       <c r="C41" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="96" t="s">
+      <c r="D41" s="62" t="s">
         <v>126</v>
       </c>
       <c r="E41" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="67"/>
+      <c r="F41" s="88"/>
       <c r="G41" s="12"/>
       <c r="H41" s="37"/>
       <c r="I41" s="3"/>
@@ -2605,13 +2628,13 @@
       <c r="C42" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="97" t="s">
+      <c r="D42" s="63" t="s">
         <v>127</v>
       </c>
       <c r="E42" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="67"/>
+      <c r="F42" s="88"/>
       <c r="G42" s="12"/>
       <c r="H42" s="37"/>
       <c r="I42" s="3"/>
@@ -2633,17 +2656,17 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" s="8" customFormat="1" ht="59.4" customHeight="1">
+    <row r="43" spans="1:26" s="8" customFormat="1" ht="41.4" customHeight="1">
       <c r="A43" s="12"/>
       <c r="B43" s="19"/>
       <c r="C43" s="21"/>
-      <c r="D43" s="97" t="s">
+      <c r="D43" s="63" t="s">
         <v>127</v>
       </c>
       <c r="E43" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="F43" s="67"/>
+      <c r="F43" s="88"/>
       <c r="G43" s="12"/>
       <c r="H43" s="37"/>
       <c r="I43" s="3"/>
@@ -2665,17 +2688,19 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
+    <row r="44" spans="1:26" s="8" customFormat="1" ht="67.2" customHeight="1">
       <c r="A44" s="12"/>
       <c r="B44" s="19"/>
       <c r="C44" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="51"/>
+      <c r="D44" s="99" t="s">
+        <v>134</v>
+      </c>
       <c r="E44" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="68"/>
+      <c r="F44" s="89"/>
       <c r="G44" s="12"/>
       <c r="H44" s="37"/>
       <c r="I44" s="3"/>
@@ -2758,22 +2783,22 @@
       <c r="Z46" s="6"/>
     </row>
     <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="69">
+      <c r="A47" s="68">
         <v>4</v>
       </c>
-      <c r="B47" s="72" t="s">
+      <c r="B47" s="71" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="75" t="s">
+      <c r="D47" s="77" t="s">
         <v>128</v>
       </c>
       <c r="E47" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="66" t="s">
+      <c r="F47" s="65" t="s">
         <v>89</v>
       </c>
       <c r="G47" s="37" t="s">
@@ -2800,16 +2825,16 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A48" s="70"/>
-      <c r="B48" s="73"/>
+      <c r="A48" s="69"/>
+      <c r="B48" s="72"/>
       <c r="C48" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="76"/>
+      <c r="D48" s="90"/>
       <c r="E48" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="F48" s="67"/>
+      <c r="F48" s="88"/>
       <c r="G48" s="38"/>
       <c r="H48" s="38"/>
       <c r="I48" s="9"/>
@@ -2832,14 +2857,14 @@
       <c r="Z48" s="9"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="70"/>
-      <c r="B49" s="73"/>
+      <c r="A49" s="69"/>
+      <c r="B49" s="72"/>
       <c r="C49" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="76"/>
-      <c r="E49" s="80"/>
-      <c r="F49" s="67"/>
+      <c r="D49" s="90"/>
+      <c r="E49" s="94"/>
+      <c r="F49" s="88"/>
       <c r="G49" s="37"/>
       <c r="H49" s="37"/>
       <c r="I49" s="3"/>
@@ -2862,12 +2887,12 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="70"/>
-      <c r="B50" s="73"/>
-      <c r="C50" s="78"/>
-      <c r="D50" s="76"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="67"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="72"/>
+      <c r="C50" s="92"/>
+      <c r="D50" s="90"/>
+      <c r="E50" s="95"/>
+      <c r="F50" s="88"/>
       <c r="G50" s="37"/>
       <c r="H50" s="37"/>
       <c r="I50" s="3"/>
@@ -2890,12 +2915,12 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A51" s="71"/>
-      <c r="B51" s="74"/>
-      <c r="C51" s="79"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="82"/>
-      <c r="F51" s="68"/>
+      <c r="A51" s="70"/>
+      <c r="B51" s="73"/>
+      <c r="C51" s="93"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="96"/>
+      <c r="F51" s="89"/>
       <c r="G51" s="37"/>
       <c r="H51" s="37"/>
       <c r="I51" s="3"/>
@@ -2946,22 +2971,22 @@
       <c r="Z52" s="6"/>
     </row>
     <row r="53" spans="1:26" s="4" customFormat="1" ht="46.8" customHeight="1">
-      <c r="A53" s="86">
+      <c r="A53" s="75">
         <v>5</v>
       </c>
-      <c r="B53" s="85" t="s">
+      <c r="B53" s="74" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="97" t="s">
+      <c r="D53" s="63" t="s">
         <v>129</v>
       </c>
       <c r="E53" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F53" s="66" t="s">
+      <c r="F53" s="65" t="s">
         <v>90</v>
       </c>
       <c r="G53" s="12"/>
@@ -2986,14 +3011,14 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="86"/>
-      <c r="B54" s="85"/>
+      <c r="A54" s="75"/>
+      <c r="B54" s="74"/>
       <c r="C54" s="21" t="s">
         <v>25</v>
       </c>
       <c r="D54" s="27"/>
       <c r="E54" s="29"/>
-      <c r="F54" s="90"/>
+      <c r="F54" s="66"/>
       <c r="G54" s="40"/>
       <c r="H54" s="37"/>
       <c r="I54" s="3"/>
@@ -3016,14 +3041,14 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A55" s="86"/>
-      <c r="B55" s="85"/>
+      <c r="A55" s="75"/>
+      <c r="B55" s="74"/>
       <c r="C55" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D55" s="27"/>
       <c r="E55" s="29"/>
-      <c r="F55" s="91"/>
+      <c r="F55" s="67"/>
       <c r="G55" s="12"/>
       <c r="H55" s="37"/>
       <c r="I55" s="3"/>
@@ -3074,20 +3099,20 @@
       <c r="Z56" s="6"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A57" s="86">
+      <c r="A57" s="75">
         <v>6</v>
       </c>
-      <c r="B57" s="85" t="s">
+      <c r="B57" s="74" t="s">
         <v>35</v>
       </c>
       <c r="C57" s="23"/>
-      <c r="D57" s="95" t="s">
+      <c r="D57" s="76" t="s">
         <v>130</v>
       </c>
       <c r="E57" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F57" s="66" t="s">
+      <c r="F57" s="65" t="s">
         <v>92</v>
       </c>
       <c r="G57" s="12"/>
@@ -3112,13 +3137,13 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A58" s="86"/>
-      <c r="B58" s="85"/>
-      <c r="D58" s="95"/>
+      <c r="A58" s="75"/>
+      <c r="B58" s="74"/>
+      <c r="D58" s="76"/>
       <c r="E58" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="F58" s="90"/>
+      <c r="F58" s="66"/>
       <c r="G58" s="40"/>
       <c r="H58" s="37"/>
       <c r="I58" s="3"/>
@@ -3141,16 +3166,16 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A59" s="86"/>
-      <c r="B59" s="85"/>
+      <c r="A59" s="75"/>
+      <c r="B59" s="74"/>
       <c r="C59" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="75"/>
+      <c r="D59" s="77"/>
       <c r="E59" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="F59" s="91"/>
+      <c r="F59" s="67"/>
       <c r="G59" s="40"/>
       <c r="H59" s="37"/>
       <c r="I59" s="3"/>
@@ -3332,21 +3357,23 @@
       <c r="Y64" s="6"/>
       <c r="Z64" s="6"/>
     </row>
-    <row r="65" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A65" s="69">
+    <row r="65" spans="1:26" s="4" customFormat="1" ht="75.599999999999994" customHeight="1">
+      <c r="A65" s="68">
         <v>8</v>
       </c>
-      <c r="B65" s="72" t="s">
+      <c r="B65" s="71" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D65" s="61"/>
+      <c r="D65" s="100" t="s">
+        <v>135</v>
+      </c>
       <c r="E65" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="66" t="s">
+      <c r="F65" s="65" t="s">
         <v>94</v>
       </c>
       <c r="G65" s="40" t="s">
@@ -3373,16 +3400,18 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="70"/>
-      <c r="B66" s="73"/>
+      <c r="A66" s="69"/>
+      <c r="B66" s="72"/>
       <c r="C66" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D66" s="61"/>
+      <c r="D66" s="100" t="s">
+        <v>136</v>
+      </c>
       <c r="E66" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="90"/>
+      <c r="F66" s="66"/>
       <c r="G66" s="40"/>
       <c r="H66" s="37"/>
       <c r="I66" s="3"/>
@@ -3405,16 +3434,18 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="70"/>
-      <c r="B67" s="73"/>
+      <c r="A67" s="69"/>
+      <c r="B67" s="72"/>
       <c r="C67" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D67" s="61"/>
+      <c r="D67" s="100" t="s">
+        <v>137</v>
+      </c>
       <c r="E67" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F67" s="90"/>
+      <c r="F67" s="66"/>
       <c r="G67" s="12"/>
       <c r="H67" s="37"/>
       <c r="I67" s="3"/>
@@ -3437,12 +3468,12 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="71"/>
-      <c r="B68" s="74"/>
+      <c r="A68" s="70"/>
+      <c r="B68" s="73"/>
       <c r="C68" s="21"/>
       <c r="D68" s="61"/>
       <c r="E68" s="20"/>
-      <c r="F68" s="91"/>
+      <c r="F68" s="67"/>
       <c r="G68" s="12"/>
       <c r="H68" s="37"/>
       <c r="I68" s="3"/>
@@ -3500,7 +3531,7 @@
         <v>50</v>
       </c>
       <c r="C70" s="21"/>
-      <c r="D70" s="98" t="s">
+      <c r="D70" s="64" t="s">
         <v>133</v>
       </c>
       <c r="E70" s="30" t="s">
@@ -3532,21 +3563,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A11:A29"/>
-    <mergeCell ref="F11:F29"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="E21:E24"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F47:F51"/>
@@ -3563,6 +3579,21 @@
     <mergeCell ref="B11:B29"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A11:A29"/>
+    <mergeCell ref="F11:F29"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
update testcases of category module
</commit_message>
<xml_diff>
--- a/Lhub_RTM.xlsx
+++ b/Lhub_RTM.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\ProjectManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="7404"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="139">
   <si>
     <t>Project Name:</t>
   </si>
@@ -211,18 +211,6 @@
   </si>
   <si>
     <t>Lhub_SRS_2.4.1.10</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.1.11</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.1.12</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.1.13</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.1.14</t>
   </si>
   <si>
     <t>Lhub_SRS_2.4.2.4</t>
@@ -426,25 +414,74 @@
     <t>resetPassword(email,password)</t>
   </si>
   <si>
-    <t>RM_1</t>
-  </si>
-  <si>
-    <t>RM_2</t>
-  </si>
-  <si>
-    <t>RM_3 , RM_4</t>
-  </si>
-  <si>
-    <t>RM_5 , RM_9 , RM_10 , RM_11 , RM_12 , RM_13</t>
-  </si>
-  <si>
-    <t>RM_6 , RM_7 , RM_14 , RM_15 , RM_16, RM_17 , RM_18 , RM_19 , RM_20 , RM_21</t>
-  </si>
-  <si>
-    <t>RM_8 , RM_22 , RM_23, RM_24 , RM_25</t>
-  </si>
-  <si>
-    <t>AM_9</t>
+    <t>update the SRS IDs column according to SRS document as SRS login module was updated</t>
+  </si>
+  <si>
+    <t>lhub_login_1</t>
+  </si>
+  <si>
+    <t>lhub_login_2</t>
+  </si>
+  <si>
+    <t>lhub_login_3</t>
+  </si>
+  <si>
+    <t>lhub_login_4</t>
+  </si>
+  <si>
+    <t>lhub_login_5</t>
+  </si>
+  <si>
+    <t>lhub_login_6</t>
+  </si>
+  <si>
+    <t>lhub_login_7</t>
+  </si>
+  <si>
+    <t>lhub_login_8</t>
+  </si>
+  <si>
+    <t>HM_17</t>
+  </si>
+  <si>
+    <t>HM_11</t>
+  </si>
+  <si>
+    <t>HM_19
+HM_20</t>
+  </si>
+  <si>
+    <t>HM_21
+HM_22
+HM_23</t>
+  </si>
+  <si>
+    <t>HM_24
+HM_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM_26
+HM_27
+HM_03
+</t>
+  </si>
+  <si>
+    <t>HM_28
+HM_29</t>
+  </si>
+  <si>
+    <t>HM_04</t>
+  </si>
+  <si>
+    <t>HM_13
+HM_14
+HM_15
+HM_16</t>
+  </si>
+  <si>
+    <t>AM_1,
+AM_2,
+AM_3 ,AM_5 ,AM_6,AM_7</t>
   </si>
   <si>
     <t>AM_1,
@@ -453,12 +490,18 @@
 AM_7</t>
   </si>
   <si>
-    <t>AM_1,
-AM_2,
-AM_3 ,AM_5 ,AM_6,AM_7</t>
-  </si>
-  <si>
     <t>AM_4 ,AM_8</t>
+  </si>
+  <si>
+    <t>AM_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat_Module_01
+Cat_Module_02
+Cat_Module_03
+Cat_Module_04
+Cat_Module_05
+</t>
   </si>
 </sst>
 </file>
@@ -472,7 +515,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -484,7 +527,7 @@
     <font>
       <sz val="16"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -519,12 +562,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -584,9 +621,16 @@
       <b/>
       <sz val="24"/>
       <color theme="0"/>
-      <name val="Calibri Light"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -770,147 +814,168 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -919,13 +984,13 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -937,90 +1002,71 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1125,22 +1171,22 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Arial">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Arial" panose="020B0604020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Hang" typeface="굴림"/>
+        <a:font script="Hans" typeface="黑体"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
         <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Cans" typeface="Euphemia"/>
@@ -1157,21 +1203,21 @@
         <a:font script="Laoo" typeface="DokChampa"/>
         <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Arial" panose="020B0604020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Hang" typeface="굴림"/>
+        <a:font script="Hans" typeface="黑体"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -1349,137 +1395,145 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:B68"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9.296875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="54.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="78.42578125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="44.5703125" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="9.28515625" style="5"/>
+    <col min="1" max="1" width="23.296875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="30.3984375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="48.296875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="28.796875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="35.59765625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="54.296875" style="20" customWidth="1"/>
+    <col min="7" max="7" width="78.3984375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="44.5" style="17" customWidth="1"/>
+    <col min="9" max="16384" width="9.296875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.900000000000006" customHeight="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="44"/>
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.95" customHeight="1">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="88"/>
+      <c r="D2" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A3" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="88"/>
+      <c r="D3" s="13">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>43588</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A4" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="14">
-        <v>1</v>
-      </c>
-      <c r="E3" s="15">
-        <v>43588</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="B4" s="89">
+        <v>43470</v>
+      </c>
+      <c r="C4" s="89"/>
+      <c r="D4" s="13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E4" s="14">
+        <v>43592</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A5" s="42"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>43601</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="46" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A4" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="82">
-        <v>43470</v>
-      </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="14">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E4" s="15">
-        <v>43592</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="14">
-        <v>1.2</v>
-      </c>
-      <c r="E5" s="15">
-        <v>43601</v>
-      </c>
-      <c r="F5" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="G5" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" s="46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-    </row>
-    <row r="7" spans="1:26" s="45" customFormat="1" ht="93" customHeight="1">
+      <c r="H5" s="45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="2" customFormat="1" ht="55.2" customHeight="1">
+      <c r="A6" s="42"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="E6" s="14">
+        <v>43608</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="45"/>
+    </row>
+    <row r="7" spans="1:26" s="44" customFormat="1" ht="93" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
@@ -1505,23 +1559,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.9" customHeight="1">
-      <c r="A8" s="84">
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.950000000000003" customHeight="1">
+      <c r="A8" s="91">
         <v>1</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="85"/>
-      <c r="E8" s="30" t="s">
+      <c r="D8" s="60"/>
+      <c r="E8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="86"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="86"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="92"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1542,18 +1596,18 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="84"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="22" t="s">
+      <c r="A9" s="91"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="85"/>
-      <c r="E9" s="30" t="s">
+      <c r="D9" s="60"/>
+      <c r="E9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="86"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="86"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="92"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1573,15 +1627,15 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.95" customHeight="1">
+      <c r="A10" s="16"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -1602,26 +1656,28 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A11" s="84">
+      <c r="A11" s="91">
         <v>2</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="30" t="s">
+      <c r="D11" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="87" t="s">
-        <v>91</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="H11" s="84"/>
+      <c r="F11" s="93" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="91"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1642,17 +1698,19 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="84"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="22" t="s">
+      <c r="A12" s="91"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="30" t="s">
+      <c r="D12" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="88"/>
-      <c r="H12" s="84"/>
+      <c r="F12" s="94"/>
+      <c r="H12" s="91"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1673,18 +1731,20 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="84"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="22" t="s">
+      <c r="A13" s="91"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="30" t="s">
+      <c r="D13" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="88"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1705,18 +1765,20 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="84"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="30" t="s">
+      <c r="A14" s="91"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="88"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1737,18 +1799,20 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="84"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="30" t="s">
+      <c r="A15" s="91"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="88"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1769,16 +1833,18 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="84"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="30" t="s">
+      <c r="A16" s="91"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="88"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1799,16 +1865,18 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="84"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="30" t="s">
+      <c r="A17" s="91"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="88"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1829,16 +1897,18 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="84"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="30" t="s">
+      <c r="A18" s="91"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="88"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1859,16 +1929,18 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="84"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="30" t="s">
+      <c r="A19" s="91"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="88"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1889,16 +1961,18 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="84"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="30" t="s">
+      <c r="A20" s="91"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="88"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1919,18 +1993,16 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="84"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="88"/>
-      <c r="G21" s="53" t="s">
-        <v>119</v>
-      </c>
-      <c r="H21" s="38"/>
+      <c r="A21" s="91"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="97"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="37"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1951,16 +2023,14 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="84"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="88"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
+      <c r="A22" s="91"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1981,16 +2051,14 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="84"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="88"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
+      <c r="A23" s="91"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2011,16 +2079,14 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="84"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="88"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
+      <c r="A24" s="91"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2041,20 +2107,18 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
-      <c r="A25" s="84"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="73" t="s">
-        <v>120</v>
-      </c>
-      <c r="E25" s="30" t="s">
+      <c r="A25" s="91"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="88"/>
-      <c r="G25" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" s="38"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="37"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2075,16 +2139,16 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="84"/>
-      <c r="B26" s="83"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="30" t="s">
+      <c r="A26" s="91"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="88"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
+      <c r="F26" s="94"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2105,16 +2169,16 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="84"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="30" t="s">
+      <c r="A27" s="91"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="88"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2135,16 +2199,16 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="84"/>
-      <c r="B28" s="83"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="88"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
+      <c r="A28" s="91"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="94"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -2165,16 +2229,16 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="84"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="88"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
+      <c r="A29" s="91"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="94"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2196,15 +2260,15 @@
     </row>
     <row r="30" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A30" s="12"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="34"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="33"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2226,15 +2290,15 @@
     </row>
     <row r="31" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A31" s="12"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="34"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="33"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2256,15 +2320,15 @@
     </row>
     <row r="32" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A32" s="12"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="34"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="33"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2284,19 +2348,17 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" s="4" customFormat="1">
+    <row r="33" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A33" s="12"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="34"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="33"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2316,19 +2378,17 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" s="4" customFormat="1" ht="54">
+    <row r="34" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A34" s="12"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="59" t="s">
-        <v>123</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F34" s="34"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="33"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2348,19 +2408,17 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" s="4" customFormat="1" ht="111.95" customHeight="1">
+    <row r="35" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
       <c r="A35" s="12"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" s="34"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35" s="33"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2380,17 +2438,17 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" s="4" customFormat="1">
+    <row r="36" spans="1:26" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A36" s="12"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="34"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="33"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2410,19 +2468,17 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" s="8" customFormat="1" ht="54">
+    <row r="37" spans="1:26" s="8" customFormat="1" ht="19.95" customHeight="1">
       <c r="A37" s="12"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="F37" s="34"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="38"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="33"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="37"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2442,19 +2498,17 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" s="8" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="38" spans="1:26" s="8" customFormat="1" ht="19.95" customHeight="1">
       <c r="A38" s="12"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="F38" s="34"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="38"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="33"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="37"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2474,15 +2528,15 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.45" customHeight="1">
-      <c r="A39" s="17"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="42"/>
+    <row r="39" spans="1:26" s="7" customFormat="1" ht="11.4" customHeight="1">
+      <c r="A39" s="16"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="41"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -2506,21 +2560,23 @@
       <c r="A40" s="12">
         <v>3</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="31" t="s">
+      <c r="D40" s="62" t="s">
+        <v>125</v>
+      </c>
+      <c r="E40" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="64" t="s">
-        <v>92</v>
+      <c r="F40" s="71" t="s">
+        <v>88</v>
       </c>
       <c r="G40" s="12"/>
-      <c r="H40" s="38"/>
+      <c r="H40" s="37"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2542,17 +2598,19 @@
     </row>
     <row r="41" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A41" s="12"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="22" t="s">
+      <c r="B41" s="19"/>
+      <c r="C41" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="28"/>
-      <c r="E41" s="31" t="s">
+      <c r="D41" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="65"/>
+      <c r="F41" s="72"/>
       <c r="G41" s="12"/>
-      <c r="H41" s="38"/>
+      <c r="H41" s="37"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2572,19 +2630,21 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
+    <row r="42" spans="1:26" s="8" customFormat="1" ht="51.6" customHeight="1">
       <c r="A42" s="12"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="22" t="s">
+      <c r="B42" s="19"/>
+      <c r="C42" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="28"/>
-      <c r="E42" s="31" t="s">
+      <c r="D42" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="65"/>
+      <c r="F42" s="72"/>
       <c r="G42" s="12"/>
-      <c r="H42" s="38"/>
+      <c r="H42" s="37"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -2604,17 +2664,19 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
+    <row r="43" spans="1:26" s="8" customFormat="1" ht="41.4" customHeight="1">
       <c r="A43" s="12"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="F43" s="65"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F43" s="72"/>
       <c r="G43" s="12"/>
-      <c r="H43" s="38"/>
+      <c r="H43" s="37"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -2634,53 +2696,53 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" s="97" customFormat="1" ht="85.5" customHeight="1">
-      <c r="A44" s="91"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="93" t="s">
+    <row r="44" spans="1:26" s="8" customFormat="1" ht="67.2" customHeight="1">
+      <c r="A44" s="12"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="93" t="s">
-        <v>128</v>
-      </c>
-      <c r="E44" s="94" t="s">
+      <c r="D44" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="66"/>
-      <c r="G44" s="91"/>
-      <c r="H44" s="95"/>
-      <c r="I44" s="96"/>
-      <c r="J44" s="96"/>
-      <c r="K44" s="96"/>
-      <c r="L44" s="96"/>
-      <c r="M44" s="96"/>
-      <c r="N44" s="96"/>
-      <c r="O44" s="96"/>
-      <c r="P44" s="96"/>
-      <c r="Q44" s="96"/>
-      <c r="R44" s="96"/>
-      <c r="S44" s="96"/>
-      <c r="T44" s="96"/>
-      <c r="U44" s="96"/>
-      <c r="V44" s="96"/>
-      <c r="W44" s="96"/>
-      <c r="X44" s="96"/>
-      <c r="Y44" s="96"/>
-      <c r="Z44" s="96"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="3"/>
+      <c r="X44" s="3"/>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3"/>
     </row>
     <row r="45" spans="1:26" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A45" s="12"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="34" t="s">
-        <v>82</v>
+      <c r="B45" s="19"/>
+      <c r="C45" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="51"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="33" t="s">
+        <v>78</v>
       </c>
       <c r="G45" s="12"/>
-      <c r="H45" s="38"/>
+      <c r="H45" s="37"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -2701,14 +2763,14 @@
       <c r="Z45" s="3"/>
     </row>
     <row r="46" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A46" s="17"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="42"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="41"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -2729,26 +2791,28 @@
       <c r="Z46" s="6"/>
     </row>
     <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="67">
+      <c r="A47" s="74">
         <v>4</v>
       </c>
-      <c r="B47" s="70" t="s">
+      <c r="B47" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="73"/>
-      <c r="E47" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="F47" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="G47" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="H47" s="38"/>
+      <c r="D47" s="80" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="F47" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="G47" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="H47" s="37"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -2769,18 +2833,18 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A48" s="68"/>
-      <c r="B48" s="71"/>
-      <c r="C48" s="25" t="s">
+      <c r="A48" s="75"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="74"/>
-      <c r="E48" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="F48" s="65"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F48" s="72"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -2801,16 +2865,16 @@
       <c r="Z48" s="9"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="68"/>
-      <c r="B49" s="71"/>
-      <c r="C49" s="22" t="s">
+      <c r="A49" s="75"/>
+      <c r="B49" s="78"/>
+      <c r="C49" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="74"/>
-      <c r="E49" s="78"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="85"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -2831,14 +2895,14 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="68"/>
-      <c r="B50" s="71"/>
-      <c r="C50" s="76"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="79"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
+      <c r="A50" s="75"/>
+      <c r="B50" s="78"/>
+      <c r="C50" s="83"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="86"/>
+      <c r="F50" s="72"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -2859,14 +2923,14 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A51" s="69"/>
-      <c r="B51" s="72"/>
-      <c r="C51" s="77"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="80"/>
-      <c r="F51" s="66"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
+      <c r="A51" s="76"/>
+      <c r="B51" s="79"/>
+      <c r="C51" s="84"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="87"/>
+      <c r="F51" s="73"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2887,14 +2951,14 @@
       <c r="Z51" s="3"/>
     </row>
     <row r="52" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A52" s="17"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="42"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="41"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -2914,25 +2978,27 @@
       <c r="Y52" s="6"/>
       <c r="Z52" s="6"/>
     </row>
-    <row r="53" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A53" s="84">
+    <row r="53" spans="1:26" s="4" customFormat="1" ht="46.8" customHeight="1">
+      <c r="A53" s="91">
         <v>5</v>
       </c>
-      <c r="B53" s="83" t="s">
+      <c r="B53" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="28"/>
-      <c r="E53" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="F53" s="64" t="s">
-        <v>94</v>
+      <c r="D53" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" s="71" t="s">
+        <v>90</v>
       </c>
       <c r="G53" s="12"/>
-      <c r="H53" s="38"/>
+      <c r="H53" s="37"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2953,16 +3019,16 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="84"/>
-      <c r="B54" s="83"/>
-      <c r="C54" s="22" t="s">
+      <c r="A54" s="91"/>
+      <c r="B54" s="90"/>
+      <c r="C54" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="28"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="89"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="38"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="95"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="37"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2983,16 +3049,16 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A55" s="84"/>
-      <c r="B55" s="83"/>
-      <c r="C55" s="22" t="s">
+      <c r="A55" s="91"/>
+      <c r="B55" s="90"/>
+      <c r="C55" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D55" s="28"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="90"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="96"/>
       <c r="G55" s="12"/>
-      <c r="H55" s="38"/>
+      <c r="H55" s="37"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -3013,14 +3079,14 @@
       <c r="Z55" s="3"/>
     </row>
     <row r="56" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1">
-      <c r="A56" s="17"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="42"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="41"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -3041,22 +3107,24 @@
       <c r="Z56" s="6"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A57" s="84">
+      <c r="A57" s="91">
         <v>6</v>
       </c>
-      <c r="B57" s="83" t="s">
+      <c r="B57" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="24"/>
-      <c r="D57" s="85"/>
-      <c r="E57" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="F57" s="64" t="s">
-        <v>96</v>
+      <c r="C57" s="23"/>
+      <c r="D57" s="100" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F57" s="71" t="s">
+        <v>92</v>
       </c>
       <c r="G57" s="12"/>
-      <c r="H57" s="38"/>
+      <c r="H57" s="37"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -3077,15 +3145,15 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A58" s="84"/>
-      <c r="B58" s="83"/>
-      <c r="D58" s="85"/>
-      <c r="E58" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="F58" s="89"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="38"/>
+      <c r="A58" s="91"/>
+      <c r="B58" s="90"/>
+      <c r="D58" s="100"/>
+      <c r="E58" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F58" s="95"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="37"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -3106,18 +3174,18 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A59" s="84"/>
-      <c r="B59" s="83"/>
-      <c r="C59" s="22" t="s">
+      <c r="A59" s="91"/>
+      <c r="B59" s="90"/>
+      <c r="C59" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="73"/>
-      <c r="E59" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="F59" s="90"/>
-      <c r="G59" s="41"/>
-      <c r="H59" s="38"/>
+      <c r="D59" s="80"/>
+      <c r="E59" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F59" s="96"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="37"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3137,17 +3205,19 @@
       <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
     </row>
-    <row r="60" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A60" s="49"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="F60" s="51"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="38"/>
+    <row r="60" spans="1:26" s="8" customFormat="1" ht="47.4" customHeight="1">
+      <c r="A60" s="48"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="E60" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" s="50"/>
+      <c r="G60" s="40"/>
+      <c r="H60" s="37"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -3167,17 +3237,19 @@
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" spans="1:26" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A61" s="49"/>
-      <c r="B61" s="48"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="50" t="s">
-        <v>113</v>
-      </c>
-      <c r="F61" s="51"/>
-      <c r="G61" s="41"/>
-      <c r="H61" s="38"/>
+    <row r="61" spans="1:26" s="8" customFormat="1" ht="69.599999999999994" customHeight="1">
+      <c r="A61" s="48"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="E61" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="F61" s="50"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="37"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -3197,15 +3269,15 @@
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
     </row>
-    <row r="62" spans="1:26" s="7" customFormat="1" ht="22.9" customHeight="1">
-      <c r="A62" s="17"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="42"/>
+    <row r="62" spans="1:26" s="7" customFormat="1" ht="22.95" customHeight="1">
+      <c r="A62" s="16"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="41"/>
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
@@ -3225,27 +3297,29 @@
       <c r="Y62" s="6"/>
       <c r="Z62" s="6"/>
     </row>
-    <row r="63" spans="1:26" s="4" customFormat="1" ht="67.900000000000006" customHeight="1">
+    <row r="63" spans="1:26" s="4" customFormat="1" ht="90" customHeight="1">
       <c r="A63" s="12">
         <v>7</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C63" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D63" s="27"/>
-      <c r="E63" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="F63" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="G63" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="H63" s="38"/>
+      <c r="C63" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D63" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="F63" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="G63" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="H63" s="37"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -3265,15 +3339,15 @@
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
     </row>
-    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.45" customHeight="1">
-      <c r="A64" s="17"/>
-      <c r="B64" s="19"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="26"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="42"/>
+    <row r="64" spans="1:26" s="7" customFormat="1" ht="20.399999999999999" customHeight="1">
+      <c r="A64" s="16"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="41"/>
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
@@ -3293,125 +3367,125 @@
       <c r="Y64" s="6"/>
       <c r="Z64" s="6"/>
     </row>
-    <row r="65" spans="1:26" s="97" customFormat="1" ht="86.25" customHeight="1">
-      <c r="A65" s="67">
+    <row r="65" spans="1:26" s="4" customFormat="1" ht="75.599999999999994" customHeight="1">
+      <c r="A65" s="74">
         <v>8</v>
       </c>
-      <c r="B65" s="70" t="s">
+      <c r="B65" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="C65" s="93" t="s">
-        <v>89</v>
-      </c>
-      <c r="D65" s="98" t="s">
-        <v>127</v>
-      </c>
-      <c r="E65" s="99" t="s">
+      <c r="C65" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D65" s="66" t="s">
+        <v>135</v>
+      </c>
+      <c r="E65" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="64" t="s">
-        <v>98</v>
-      </c>
-      <c r="G65" s="100" t="s">
-        <v>118</v>
-      </c>
-      <c r="H65" s="95"/>
-      <c r="I65" s="96"/>
-      <c r="J65" s="96"/>
-      <c r="K65" s="96"/>
-      <c r="L65" s="96"/>
-      <c r="M65" s="96"/>
-      <c r="N65" s="96"/>
-      <c r="O65" s="96"/>
-      <c r="P65" s="96"/>
-      <c r="Q65" s="96"/>
-      <c r="R65" s="96"/>
-      <c r="S65" s="96"/>
-      <c r="T65" s="96"/>
-      <c r="U65" s="96"/>
-      <c r="V65" s="96"/>
-      <c r="W65" s="96"/>
-      <c r="X65" s="96"/>
-      <c r="Y65" s="96"/>
-      <c r="Z65" s="96"/>
-    </row>
-    <row r="66" spans="1:26" s="97" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="68"/>
-      <c r="B66" s="71"/>
-      <c r="C66" s="93" t="s">
-        <v>86</v>
-      </c>
-      <c r="D66" s="98" t="s">
-        <v>129</v>
-      </c>
-      <c r="E66" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="F66" s="89"/>
-      <c r="G66" s="100"/>
-      <c r="H66" s="95"/>
-      <c r="I66" s="96"/>
-      <c r="J66" s="96"/>
-      <c r="K66" s="96"/>
-      <c r="L66" s="96"/>
-      <c r="M66" s="96"/>
-      <c r="N66" s="96"/>
-      <c r="O66" s="96"/>
-      <c r="P66" s="96"/>
-      <c r="Q66" s="96"/>
-      <c r="R66" s="96"/>
-      <c r="S66" s="96"/>
-      <c r="T66" s="96"/>
-      <c r="U66" s="96"/>
-      <c r="V66" s="96"/>
-      <c r="W66" s="96"/>
-      <c r="X66" s="96"/>
-      <c r="Y66" s="96"/>
-      <c r="Z66" s="96"/>
-    </row>
-    <row r="67" spans="1:26" s="97" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="68"/>
-      <c r="B67" s="71"/>
-      <c r="C67" s="93" t="s">
-        <v>85</v>
-      </c>
-      <c r="D67" s="98" t="s">
-        <v>126</v>
-      </c>
-      <c r="E67" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="F67" s="89"/>
-      <c r="G67" s="91"/>
-      <c r="H67" s="95"/>
-      <c r="I67" s="96"/>
-      <c r="J67" s="96"/>
-      <c r="K67" s="96"/>
-      <c r="L67" s="96"/>
-      <c r="M67" s="96"/>
-      <c r="N67" s="96"/>
-      <c r="O67" s="96"/>
-      <c r="P67" s="96"/>
-      <c r="Q67" s="96"/>
-      <c r="R67" s="96"/>
-      <c r="S67" s="96"/>
-      <c r="T67" s="96"/>
-      <c r="U67" s="96"/>
-      <c r="V67" s="96"/>
-      <c r="W67" s="96"/>
-      <c r="X67" s="96"/>
-      <c r="Y67" s="96"/>
-      <c r="Z67" s="96"/>
+      <c r="F65" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="G65" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="H65" s="37"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="3"/>
+      <c r="V65" s="3"/>
+      <c r="W65" s="3"/>
+      <c r="X65" s="3"/>
+      <c r="Y65" s="3"/>
+      <c r="Z65" s="3"/>
+    </row>
+    <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A66" s="75"/>
+      <c r="B66" s="78"/>
+      <c r="C66" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D66" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F66" s="95"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3"/>
+      <c r="U66" s="3"/>
+      <c r="V66" s="3"/>
+      <c r="W66" s="3"/>
+      <c r="X66" s="3"/>
+      <c r="Y66" s="3"/>
+      <c r="Z66" s="3"/>
+    </row>
+    <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A67" s="75"/>
+      <c r="B67" s="78"/>
+      <c r="C67" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D67" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F67" s="95"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
+      <c r="V67" s="3"/>
+      <c r="W67" s="3"/>
+      <c r="X67" s="3"/>
+      <c r="Y67" s="3"/>
+      <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="69"/>
-      <c r="B68" s="72"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="90"/>
+      <c r="A68" s="76"/>
+      <c r="B68" s="79"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="61"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="96"/>
       <c r="G68" s="12"/>
-      <c r="H68" s="38"/>
+      <c r="H68" s="37"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -3431,15 +3505,15 @@
       <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
     </row>
-    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.149999999999999" customHeight="1">
-      <c r="A69" s="17"/>
-      <c r="B69" s="19"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="26"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="42"/>
+    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.2" customHeight="1">
+      <c r="A69" s="16"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="41"/>
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
@@ -3459,23 +3533,25 @@
       <c r="Y69" s="6"/>
       <c r="Z69" s="6"/>
     </row>
-    <row r="70" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
+    <row r="70" spans="1:26" s="4" customFormat="1" ht="91.2" customHeight="1">
       <c r="A70" s="12">
         <v>9</v>
       </c>
-      <c r="B70" s="21" t="s">
+      <c r="B70" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C70" s="22"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="F70" s="36" t="s">
-        <v>97</v>
+      <c r="C70" s="21"/>
+      <c r="D70" s="64" t="s">
+        <v>133</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F70" s="35" t="s">
+        <v>93</v>
       </c>
       <c r="G70" s="12"/>
-      <c r="H70" s="38"/>
+      <c r="H70" s="37"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -3496,9 +3572,7 @@
       <c r="Z70" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="F53:F55"/>
+  <mergeCells count="31">
     <mergeCell ref="F57:F59"/>
     <mergeCell ref="F65:F68"/>
     <mergeCell ref="A65:A68"/>
@@ -3506,14 +3580,14 @@
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="D57:D59"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="A11:A29"/>
     <mergeCell ref="F11:F29"/>
-    <mergeCell ref="D25:D32"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="E21:E24"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F47:F51"/>
@@ -3529,7 +3603,7 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B11:B29"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
update rtm with category module testcases
</commit_message>
<xml_diff>
--- a/Lhub_RTM.xlsx
+++ b/Lhub_RTM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI subjects\software project management\project 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\ProjectManagement\project\Learning-hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="139">
   <si>
     <t>Project Name:</t>
   </si>
@@ -494,6 +494,14 @@
   </si>
   <si>
     <t>AM_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat_Module_01
+Cat_Module_02
+Cat_Module_03
+Cat_Module_04
+Cat_Module_05
+</t>
   </si>
 </sst>
 </file>
@@ -778,7 +786,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -958,14 +966,35 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -985,52 +1014,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1054,10 +1038,37 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1388,7 +1399,7 @@
   <dimension ref="A1:Z70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.296875" defaultRowHeight="17.399999999999999"/>
@@ -1408,21 +1419,21 @@
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
       <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="97"/>
+      <c r="C2" s="89"/>
       <c r="D2" s="59" t="s">
         <v>51</v>
       </c>
@@ -1443,10 +1454,10 @@
       <c r="A3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="97"/>
+      <c r="C3" s="89"/>
       <c r="D3" s="13">
         <v>1</v>
       </c>
@@ -1467,10 +1478,10 @@
       <c r="A4" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="98">
+      <c r="B4" s="90">
         <v>43470</v>
       </c>
-      <c r="C4" s="98"/>
+      <c r="C4" s="90"/>
       <c r="D4" s="13">
         <v>1.1000000000000001</v>
       </c>
@@ -1489,8 +1500,8 @@
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A5" s="42"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="87"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="13">
         <v>1.2</v>
       </c>
@@ -1552,10 +1563,10 @@
       </c>
     </row>
     <row r="8" spans="1:26" s="4" customFormat="1" ht="37.950000000000003" customHeight="1">
-      <c r="A8" s="75">
+      <c r="A8" s="92">
         <v>1</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="91" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -1565,9 +1576,9 @@
       <c r="E8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="78"/>
+      <c r="F8" s="93"/>
       <c r="G8" s="36"/>
-      <c r="H8" s="78"/>
+      <c r="H8" s="93"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1588,8 +1599,8 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="75"/>
-      <c r="B9" s="74"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
@@ -1597,9 +1608,9 @@
       <c r="E9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="78"/>
+      <c r="F9" s="93"/>
       <c r="G9" s="36"/>
-      <c r="H9" s="78"/>
+      <c r="H9" s="93"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1648,10 +1659,10 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A11" s="75">
+      <c r="A11" s="92">
         <v>2</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="91" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="21" t="s">
@@ -1663,13 +1674,13 @@
       <c r="E11" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="79" t="s">
+      <c r="F11" s="94" t="s">
         <v>87</v>
       </c>
       <c r="G11" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="H11" s="75"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1690,8 +1701,8 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="75"/>
-      <c r="B12" s="74"/>
+      <c r="A12" s="92"/>
+      <c r="B12" s="91"/>
       <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
@@ -1701,8 +1712,8 @@
       <c r="E12" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="80"/>
-      <c r="H12" s="75"/>
+      <c r="F12" s="95"/>
+      <c r="H12" s="92"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1723,8 +1734,8 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="75"/>
-      <c r="B13" s="74"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="91"/>
       <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
@@ -1734,7 +1745,7 @@
       <c r="E13" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="80"/>
+      <c r="F13" s="95"/>
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="3"/>
@@ -1757,8 +1768,8 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="75"/>
-      <c r="B14" s="74"/>
+      <c r="A14" s="92"/>
+      <c r="B14" s="91"/>
       <c r="C14" s="21" t="s">
         <v>83</v>
       </c>
@@ -1768,7 +1779,7 @@
       <c r="E14" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="80"/>
+      <c r="F14" s="95"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="3"/>
@@ -1791,8 +1802,8 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="75"/>
-      <c r="B15" s="74"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="91"/>
       <c r="C15" s="21" t="s">
         <v>80</v>
       </c>
@@ -1802,7 +1813,7 @@
       <c r="E15" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="80"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="3"/>
@@ -1825,8 +1836,8 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="75"/>
-      <c r="B16" s="74"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="91"/>
       <c r="C16" s="23"/>
       <c r="D16" s="60" t="s">
         <v>117</v>
@@ -1834,7 +1845,7 @@
       <c r="E16" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="80"/>
+      <c r="F16" s="95"/>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="3"/>
@@ -1857,8 +1868,8 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="75"/>
-      <c r="B17" s="74"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="91"/>
       <c r="C17" s="23"/>
       <c r="D17" s="60" t="s">
         <v>122</v>
@@ -1866,7 +1877,7 @@
       <c r="E17" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="80"/>
+      <c r="F17" s="95"/>
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="3"/>
@@ -1889,8 +1900,8 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="75"/>
-      <c r="B18" s="74"/>
+      <c r="A18" s="92"/>
+      <c r="B18" s="91"/>
       <c r="C18" s="23"/>
       <c r="D18" s="60" t="s">
         <v>123</v>
@@ -1898,7 +1909,7 @@
       <c r="E18" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="80"/>
+      <c r="F18" s="95"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="3"/>
@@ -1921,8 +1932,8 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="75"/>
-      <c r="B19" s="74"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="91"/>
       <c r="C19" s="23"/>
       <c r="D19" s="60" t="s">
         <v>117</v>
@@ -1930,7 +1941,7 @@
       <c r="E19" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="80"/>
+      <c r="F19" s="95"/>
       <c r="G19" s="37"/>
       <c r="H19" s="37"/>
       <c r="I19" s="3"/>
@@ -1953,8 +1964,8 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="75"/>
-      <c r="B20" s="74"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="91"/>
       <c r="C20" s="23"/>
       <c r="D20" s="60" t="s">
         <v>124</v>
@@ -1962,7 +1973,7 @@
       <c r="E20" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="80"/>
+      <c r="F20" s="95"/>
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
       <c r="I20" s="3"/>
@@ -1985,12 +1996,12 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="75"/>
-      <c r="B21" s="74"/>
+      <c r="A21" s="92"/>
+      <c r="B21" s="91"/>
       <c r="C21" s="23"/>
       <c r="D21" s="60"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="80"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="95"/>
       <c r="G21" s="52" t="s">
         <v>115</v>
       </c>
@@ -2015,12 +2026,12 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="75"/>
-      <c r="B22" s="74"/>
+      <c r="A22" s="92"/>
+      <c r="B22" s="91"/>
       <c r="C22" s="23"/>
       <c r="D22" s="60"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="80"/>
+      <c r="E22" s="99"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
       <c r="I22" s="3"/>
@@ -2043,12 +2054,12 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="75"/>
-      <c r="B23" s="74"/>
+      <c r="A23" s="92"/>
+      <c r="B23" s="91"/>
       <c r="C23" s="23"/>
       <c r="D23" s="60"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="80"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="95"/>
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
       <c r="I23" s="3"/>
@@ -2071,12 +2082,12 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="75"/>
-      <c r="B24" s="74"/>
+      <c r="A24" s="92"/>
+      <c r="B24" s="91"/>
       <c r="C24" s="23"/>
       <c r="D24" s="60"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="80"/>
+      <c r="E24" s="100"/>
+      <c r="F24" s="95"/>
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
       <c r="I24" s="3"/>
@@ -2099,14 +2110,14 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
-      <c r="A25" s="75"/>
-      <c r="B25" s="74"/>
+      <c r="A25" s="92"/>
+      <c r="B25" s="91"/>
       <c r="C25" s="23"/>
       <c r="D25" s="60"/>
       <c r="E25" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="80"/>
+      <c r="F25" s="95"/>
       <c r="G25" s="56" t="s">
         <v>112</v>
       </c>
@@ -2131,14 +2142,14 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="75"/>
-      <c r="B26" s="74"/>
+      <c r="A26" s="92"/>
+      <c r="B26" s="91"/>
       <c r="C26" s="23"/>
       <c r="D26" s="60"/>
       <c r="E26" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="80"/>
+      <c r="F26" s="95"/>
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
       <c r="I26" s="3"/>
@@ -2161,14 +2172,14 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="75"/>
-      <c r="B27" s="74"/>
+      <c r="A27" s="92"/>
+      <c r="B27" s="91"/>
       <c r="C27" s="23"/>
       <c r="D27" s="60"/>
       <c r="E27" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="80"/>
+      <c r="F27" s="95"/>
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
       <c r="I27" s="3"/>
@@ -2191,14 +2202,14 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="75"/>
-      <c r="B28" s="74"/>
+      <c r="A28" s="92"/>
+      <c r="B28" s="91"/>
       <c r="C28" s="23"/>
       <c r="D28" s="60"/>
       <c r="E28" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="80"/>
+      <c r="F28" s="95"/>
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
       <c r="I28" s="3"/>
@@ -2221,14 +2232,14 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="75"/>
-      <c r="B29" s="74"/>
+      <c r="A29" s="92"/>
+      <c r="B29" s="91"/>
       <c r="C29" s="23"/>
       <c r="D29" s="60"/>
       <c r="E29" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="80"/>
+      <c r="F29" s="95"/>
       <c r="G29" s="37"/>
       <c r="H29" s="37"/>
       <c r="I29" s="3"/>
@@ -2564,7 +2575,7 @@
       <c r="E40" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="65" t="s">
+      <c r="F40" s="72" t="s">
         <v>88</v>
       </c>
       <c r="G40" s="12"/>
@@ -2600,7 +2611,7 @@
       <c r="E41" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="88"/>
+      <c r="F41" s="73"/>
       <c r="G41" s="12"/>
       <c r="H41" s="37"/>
       <c r="I41" s="3"/>
@@ -2634,7 +2645,7 @@
       <c r="E42" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="88"/>
+      <c r="F42" s="73"/>
       <c r="G42" s="12"/>
       <c r="H42" s="37"/>
       <c r="I42" s="3"/>
@@ -2666,7 +2677,7 @@
       <c r="E43" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="F43" s="88"/>
+      <c r="F43" s="73"/>
       <c r="G43" s="12"/>
       <c r="H43" s="37"/>
       <c r="I43" s="3"/>
@@ -2694,13 +2705,13 @@
       <c r="C44" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="99" t="s">
+      <c r="D44" s="66" t="s">
         <v>134</v>
       </c>
       <c r="E44" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="89"/>
+      <c r="F44" s="74"/>
       <c r="G44" s="12"/>
       <c r="H44" s="37"/>
       <c r="I44" s="3"/>
@@ -2783,22 +2794,22 @@
       <c r="Z46" s="6"/>
     </row>
     <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="68">
+      <c r="A47" s="75">
         <v>4</v>
       </c>
-      <c r="B47" s="71" t="s">
+      <c r="B47" s="78" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="77" t="s">
+      <c r="D47" s="81" t="s">
         <v>128</v>
       </c>
       <c r="E47" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="65" t="s">
+      <c r="F47" s="72" t="s">
         <v>89</v>
       </c>
       <c r="G47" s="37" t="s">
@@ -2825,16 +2836,16 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A48" s="69"/>
-      <c r="B48" s="72"/>
+      <c r="A48" s="76"/>
+      <c r="B48" s="79"/>
       <c r="C48" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="90"/>
+      <c r="D48" s="82"/>
       <c r="E48" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="F48" s="88"/>
+      <c r="F48" s="73"/>
       <c r="G48" s="38"/>
       <c r="H48" s="38"/>
       <c r="I48" s="9"/>
@@ -2857,14 +2868,14 @@
       <c r="Z48" s="9"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="69"/>
-      <c r="B49" s="72"/>
+      <c r="A49" s="76"/>
+      <c r="B49" s="79"/>
       <c r="C49" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="90"/>
-      <c r="E49" s="94"/>
-      <c r="F49" s="88"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="86"/>
+      <c r="F49" s="73"/>
       <c r="G49" s="37"/>
       <c r="H49" s="37"/>
       <c r="I49" s="3"/>
@@ -2887,12 +2898,12 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="69"/>
-      <c r="B50" s="72"/>
-      <c r="C50" s="92"/>
-      <c r="D50" s="90"/>
-      <c r="E50" s="95"/>
-      <c r="F50" s="88"/>
+      <c r="A50" s="76"/>
+      <c r="B50" s="79"/>
+      <c r="C50" s="84"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="87"/>
+      <c r="F50" s="73"/>
       <c r="G50" s="37"/>
       <c r="H50" s="37"/>
       <c r="I50" s="3"/>
@@ -2915,12 +2926,12 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A51" s="70"/>
-      <c r="B51" s="73"/>
-      <c r="C51" s="93"/>
-      <c r="D51" s="91"/>
-      <c r="E51" s="96"/>
-      <c r="F51" s="89"/>
+      <c r="A51" s="77"/>
+      <c r="B51" s="80"/>
+      <c r="C51" s="85"/>
+      <c r="D51" s="83"/>
+      <c r="E51" s="88"/>
+      <c r="F51" s="74"/>
       <c r="G51" s="37"/>
       <c r="H51" s="37"/>
       <c r="I51" s="3"/>
@@ -2971,10 +2982,10 @@
       <c r="Z52" s="6"/>
     </row>
     <row r="53" spans="1:26" s="4" customFormat="1" ht="46.8" customHeight="1">
-      <c r="A53" s="75">
+      <c r="A53" s="92">
         <v>5</v>
       </c>
-      <c r="B53" s="74" t="s">
+      <c r="B53" s="91" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="21" t="s">
@@ -2986,7 +2997,7 @@
       <c r="E53" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F53" s="65" t="s">
+      <c r="F53" s="72" t="s">
         <v>90</v>
       </c>
       <c r="G53" s="12"/>
@@ -3011,14 +3022,14 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="75"/>
-      <c r="B54" s="74"/>
+      <c r="A54" s="92"/>
+      <c r="B54" s="91"/>
       <c r="C54" s="21" t="s">
         <v>25</v>
       </c>
       <c r="D54" s="27"/>
       <c r="E54" s="29"/>
-      <c r="F54" s="66"/>
+      <c r="F54" s="96"/>
       <c r="G54" s="40"/>
       <c r="H54" s="37"/>
       <c r="I54" s="3"/>
@@ -3041,14 +3052,14 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A55" s="75"/>
-      <c r="B55" s="74"/>
+      <c r="A55" s="92"/>
+      <c r="B55" s="91"/>
       <c r="C55" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D55" s="27"/>
       <c r="E55" s="29"/>
-      <c r="F55" s="67"/>
+      <c r="F55" s="97"/>
       <c r="G55" s="12"/>
       <c r="H55" s="37"/>
       <c r="I55" s="3"/>
@@ -3099,20 +3110,20 @@
       <c r="Z56" s="6"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A57" s="75">
+      <c r="A57" s="92">
         <v>6</v>
       </c>
-      <c r="B57" s="74" t="s">
+      <c r="B57" s="91" t="s">
         <v>35</v>
       </c>
       <c r="C57" s="23"/>
-      <c r="D57" s="76" t="s">
+      <c r="D57" s="101" t="s">
         <v>130</v>
       </c>
       <c r="E57" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F57" s="65" t="s">
+      <c r="F57" s="72" t="s">
         <v>92</v>
       </c>
       <c r="G57" s="12"/>
@@ -3137,13 +3148,13 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A58" s="75"/>
-      <c r="B58" s="74"/>
-      <c r="D58" s="76"/>
+      <c r="A58" s="92"/>
+      <c r="B58" s="91"/>
+      <c r="D58" s="101"/>
       <c r="E58" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="F58" s="66"/>
+      <c r="F58" s="96"/>
       <c r="G58" s="40"/>
       <c r="H58" s="37"/>
       <c r="I58" s="3"/>
@@ -3166,16 +3177,16 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A59" s="75"/>
-      <c r="B59" s="74"/>
+      <c r="A59" s="92"/>
+      <c r="B59" s="91"/>
       <c r="C59" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="77"/>
+      <c r="D59" s="81"/>
       <c r="E59" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="F59" s="67"/>
+      <c r="F59" s="97"/>
       <c r="G59" s="40"/>
       <c r="H59" s="37"/>
       <c r="I59" s="3"/>
@@ -3289,7 +3300,7 @@
       <c r="Y62" s="6"/>
       <c r="Z62" s="6"/>
     </row>
-    <row r="63" spans="1:26" s="4" customFormat="1" ht="67.95" customHeight="1">
+    <row r="63" spans="1:26" s="4" customFormat="1" ht="145.80000000000001" customHeight="1">
       <c r="A63" s="12">
         <v>7</v>
       </c>
@@ -3299,7 +3310,9 @@
       <c r="C63" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D63" s="61"/>
+      <c r="D63" s="65" t="s">
+        <v>138</v>
+      </c>
       <c r="E63" s="32" t="s">
         <v>97</v>
       </c>
@@ -3358,22 +3371,22 @@
       <c r="Z64" s="6"/>
     </row>
     <row r="65" spans="1:26" s="4" customFormat="1" ht="75.599999999999994" customHeight="1">
-      <c r="A65" s="68">
+      <c r="A65" s="75">
         <v>8</v>
       </c>
-      <c r="B65" s="71" t="s">
+      <c r="B65" s="78" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D65" s="100" t="s">
+      <c r="D65" s="67" t="s">
         <v>135</v>
       </c>
       <c r="E65" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="65" t="s">
+      <c r="F65" s="72" t="s">
         <v>94</v>
       </c>
       <c r="G65" s="40" t="s">
@@ -3400,18 +3413,18 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="69"/>
-      <c r="B66" s="72"/>
+      <c r="A66" s="76"/>
+      <c r="B66" s="79"/>
       <c r="C66" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D66" s="100" t="s">
+      <c r="D66" s="67" t="s">
         <v>136</v>
       </c>
       <c r="E66" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="66"/>
+      <c r="F66" s="96"/>
       <c r="G66" s="40"/>
       <c r="H66" s="37"/>
       <c r="I66" s="3"/>
@@ -3434,18 +3447,18 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="69"/>
-      <c r="B67" s="72"/>
+      <c r="A67" s="76"/>
+      <c r="B67" s="79"/>
       <c r="C67" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D67" s="100" t="s">
+      <c r="D67" s="67" t="s">
         <v>137</v>
       </c>
       <c r="E67" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F67" s="66"/>
+      <c r="F67" s="96"/>
       <c r="G67" s="12"/>
       <c r="H67" s="37"/>
       <c r="I67" s="3"/>
@@ -3468,12 +3481,12 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="70"/>
-      <c r="B68" s="73"/>
+      <c r="A68" s="77"/>
+      <c r="B68" s="80"/>
       <c r="C68" s="21"/>
       <c r="D68" s="61"/>
       <c r="E68" s="20"/>
-      <c r="F68" s="67"/>
+      <c r="F68" s="97"/>
       <c r="G68" s="12"/>
       <c r="H68" s="37"/>
       <c r="I68" s="3"/>
@@ -3563,6 +3576,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A11:A29"/>
+    <mergeCell ref="F11:F29"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="E21:E24"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F47:F51"/>
@@ -3579,21 +3607,6 @@
     <mergeCell ref="B11:B29"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A11:A29"/>
-    <mergeCell ref="F11:F29"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
Registration Module test cases ID's have been added to the RTM
</commit_message>
<xml_diff>
--- a/Lhub_RTM.xlsx
+++ b/Lhub_RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\ProjectManagement\project\Learning-hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazmy\Documents\GitHub\Project\Learning-hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="7404"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23000" windowHeight="7400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="145">
   <si>
     <t>Project Name:</t>
   </si>
@@ -502,6 +502,24 @@
 Cat_Module_04
 Cat_Module_05
 </t>
+  </si>
+  <si>
+    <t>RM_1</t>
+  </si>
+  <si>
+    <t>RM_3 , RM_4</t>
+  </si>
+  <si>
+    <t>RM_5 , RM_9 , RM_10 , RM_11 , RM_12 , RM_13</t>
+  </si>
+  <si>
+    <t>RM_6 , RM_7 , RM_14 , RM_15 , RM_16, RM_17 , RM_18 , RM_19 , RM_20 , RM_21</t>
+  </si>
+  <si>
+    <t>RM_8 , RM_22 , RM_23, RM_24 , RM_25</t>
+  </si>
+  <si>
+    <t>RM_2</t>
   </si>
 </sst>
 </file>
@@ -786,7 +804,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -851,9 +869,6 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -975,6 +990,66 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -987,34 +1062,10 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1038,38 +1089,8 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1398,66 +1419,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.296875" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="17.5"/>
   <cols>
-    <col min="1" max="1" width="23.296875" style="17" customWidth="1"/>
-    <col min="2" max="2" width="30.3984375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="48.296875" style="17" customWidth="1"/>
-    <col min="4" max="4" width="28.796875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="35.59765625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="54.296875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="78.3984375" style="17" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="30.4140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="35.58203125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="54.33203125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="78.4140625" style="17" customWidth="1"/>
     <col min="8" max="8" width="44.5" style="17" customWidth="1"/>
-    <col min="9" max="16384" width="9.296875" style="5"/>
+    <col min="9" max="16384" width="9.33203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="73.95" customHeight="1">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="74" customHeight="1">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="87" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="43"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="59" t="s">
+      <c r="C2" s="100"/>
+      <c r="D2" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="58" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="89"/>
+      <c r="C3" s="100"/>
       <c r="D3" s="13">
         <v>1</v>
       </c>
@@ -1467,21 +1488,21 @@
       <c r="F3" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="44" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="90">
+      <c r="B4" s="101">
         <v>43470</v>
       </c>
-      <c r="C4" s="90"/>
+      <c r="C4" s="101"/>
       <c r="D4" s="13">
         <v>1.1000000000000001</v>
       </c>
@@ -1491,52 +1512,52 @@
       <c r="F4" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="44" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="71"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="90"/>
       <c r="D5" s="13">
         <v>1.2</v>
       </c>
       <c r="E5" s="14">
         <v>43601</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="44" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="2" customFormat="1" ht="55.2" customHeight="1">
-      <c r="A6" s="42"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="54"/>
+    <row r="6" spans="1:26" s="2" customFormat="1" ht="55.25" customHeight="1">
+      <c r="A6" s="41"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="13">
         <v>1.3</v>
       </c>
       <c r="E6" s="14">
         <v>43608</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="H6" s="45"/>
-    </row>
-    <row r="7" spans="1:26" s="44" customFormat="1" ht="93" customHeight="1">
+      <c r="H6" s="44"/>
+    </row>
+    <row r="7" spans="1:26" s="43" customFormat="1" ht="93" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
@@ -1562,23 +1583,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="4" customFormat="1" ht="37.950000000000003" customHeight="1">
-      <c r="A8" s="92">
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="38" customHeight="1">
+      <c r="A8" s="78">
         <v>1</v>
       </c>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="77" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="60"/>
-      <c r="E8" s="29" t="s">
+      <c r="D8" s="59"/>
+      <c r="E8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="93"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="93"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="81"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1598,19 +1619,19 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.6" customHeight="1">
-      <c r="A9" s="92"/>
-      <c r="B9" s="91"/>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="27.65" customHeight="1">
+      <c r="A9" s="78"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="29" t="s">
+      <c r="D9" s="59"/>
+      <c r="E9" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="93"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="93"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="81"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1630,7 +1651,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" ht="13.95" customHeight="1">
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="14" customHeight="1">
       <c r="A10" s="16"/>
       <c r="B10" s="18"/>
       <c r="C10" s="22"/>
@@ -1659,28 +1680,28 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A11" s="92">
+      <c r="A11" s="78">
         <v>2</v>
       </c>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="77" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="94" t="s">
+      <c r="F11" s="82" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="55" t="s">
+      <c r="G11" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="H11" s="92"/>
+      <c r="H11" s="78"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1701,19 +1722,19 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A12" s="92"/>
-      <c r="B12" s="91"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="95"/>
-      <c r="H12" s="92"/>
+      <c r="F12" s="83"/>
+      <c r="H12" s="78"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1734,20 +1755,20 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="92"/>
-      <c r="B13" s="91"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="95"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1768,20 +1789,20 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="92"/>
-      <c r="B14" s="91"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="95"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1802,20 +1823,20 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="92"/>
-      <c r="B15" s="91"/>
+      <c r="A15" s="78"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="95"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1836,18 +1857,18 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="92"/>
-      <c r="B16" s="91"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="95"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1868,18 +1889,18 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="92"/>
-      <c r="B17" s="91"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="77"/>
       <c r="C17" s="23"/>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="95"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1900,18 +1921,18 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="92"/>
-      <c r="B18" s="91"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="23"/>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="95"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1932,18 +1953,18 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="92"/>
-      <c r="B19" s="91"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="23"/>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="95"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1964,18 +1985,18 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="92"/>
-      <c r="B20" s="91"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="23"/>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="E20" s="57" t="s">
+      <c r="E20" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="95"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1996,16 +2017,16 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="92"/>
-      <c r="B21" s="91"/>
+      <c r="A21" s="78"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="23"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="52" t="s">
+      <c r="D21" s="59"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="H21" s="37"/>
+      <c r="H21" s="36"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -2026,14 +2047,14 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="92"/>
-      <c r="B22" s="91"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="23"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="99"/>
-      <c r="F22" s="95"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -2054,14 +2075,14 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="92"/>
-      <c r="B23" s="91"/>
+      <c r="A23" s="78"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="23"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="99"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2082,14 +2103,14 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="92"/>
-      <c r="B24" s="91"/>
+      <c r="A24" s="78"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="23"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2109,19 +2130,21 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1">
-      <c r="A25" s="92"/>
-      <c r="B25" s="91"/>
+    <row r="25" spans="1:26" s="4" customFormat="1" ht="35">
+      <c r="A25" s="78"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="23"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="29" t="s">
+      <c r="D25" s="80" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="95"/>
-      <c r="G25" s="56" t="s">
+      <c r="F25" s="83"/>
+      <c r="G25" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="H25" s="37"/>
+      <c r="H25" s="36"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2141,17 +2164,17 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="92"/>
-      <c r="B26" s="91"/>
+    <row r="26" spans="1:26" s="4" customFormat="1">
+      <c r="A26" s="78"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="23"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="29" t="s">
+      <c r="D26" s="93"/>
+      <c r="E26" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="95"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2171,17 +2194,17 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="92"/>
-      <c r="B27" s="91"/>
+    <row r="27" spans="1:26" s="4" customFormat="1">
+      <c r="A27" s="78"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="23"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="29" t="s">
+      <c r="D27" s="93"/>
+      <c r="E27" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="95"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2201,17 +2224,17 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="92"/>
-      <c r="B28" s="91"/>
+    <row r="28" spans="1:26" s="4" customFormat="1">
+      <c r="A28" s="78"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="23"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="29" t="s">
+      <c r="D28" s="93"/>
+      <c r="E28" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="95"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -2231,17 +2254,17 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="92"/>
-      <c r="B29" s="91"/>
+    <row r="29" spans="1:26" s="4" customFormat="1">
+      <c r="A29" s="78"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="23"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="29" t="s">
+      <c r="D29" s="93"/>
+      <c r="E29" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="95"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
+      <c r="F29" s="83"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2261,17 +2284,17 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="30" spans="1:26" s="4" customFormat="1">
       <c r="A30" s="12"/>
       <c r="B30" s="19"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="29" t="s">
+      <c r="D30" s="93"/>
+      <c r="E30" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="33"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2291,17 +2314,17 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="31" spans="1:26" s="4" customFormat="1">
       <c r="A31" s="12"/>
       <c r="B31" s="19"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="29" t="s">
+      <c r="D31" s="93"/>
+      <c r="E31" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2321,17 +2344,17 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="32" spans="1:26" s="4" customFormat="1">
       <c r="A32" s="12"/>
       <c r="B32" s="19"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="29" t="s">
+      <c r="D32" s="94"/>
+      <c r="E32" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2351,17 +2374,19 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="33" spans="1:26" s="4" customFormat="1">
       <c r="A33" s="12"/>
       <c r="B33" s="19"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="29" t="s">
+      <c r="D33" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="33"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2381,17 +2406,19 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="34" spans="1:26" s="4" customFormat="1" ht="35">
       <c r="A34" s="12"/>
       <c r="B34" s="19"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="29" t="s">
+      <c r="D34" s="102" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F34" s="33"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2411,17 +2438,19 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1">
+    <row r="35" spans="1:26" s="4" customFormat="1">
       <c r="A35" s="12"/>
       <c r="B35" s="19"/>
       <c r="C35" s="21"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="29" t="s">
+      <c r="D35" s="80" t="s">
+        <v>142</v>
+      </c>
+      <c r="E35" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="F35" s="33"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2441,17 +2470,17 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" s="4" customFormat="1" ht="19.95" customHeight="1">
+    <row r="36" spans="1:26" s="4" customFormat="1">
       <c r="A36" s="12"/>
       <c r="B36" s="19"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="29" t="s">
+      <c r="D36" s="94"/>
+      <c r="E36" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="33"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2471,17 +2500,19 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" s="8" customFormat="1" ht="19.95" customHeight="1">
+    <row r="37" spans="1:26" s="8" customFormat="1" ht="35">
       <c r="A37" s="12"/>
       <c r="B37" s="19"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="29" t="s">
+      <c r="D37" s="67" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="F37" s="33"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="37"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="36"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2501,17 +2532,19 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" s="8" customFormat="1" ht="19.95" customHeight="1">
+    <row r="38" spans="1:26" s="8" customFormat="1">
       <c r="A38" s="12"/>
       <c r="B38" s="19"/>
       <c r="C38" s="21"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="29" t="s">
+      <c r="D38" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="F38" s="33"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="37"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="36"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2537,9 +2570,9 @@
       <c r="C39" s="22"/>
       <c r="D39" s="25"/>
       <c r="E39" s="18"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="41"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="40"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -2569,17 +2602,17 @@
       <c r="C40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="62" t="s">
+      <c r="D40" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="E40" s="30" t="s">
+      <c r="E40" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="72" t="s">
+      <c r="F40" s="68" t="s">
         <v>88</v>
       </c>
       <c r="G40" s="12"/>
-      <c r="H40" s="37"/>
+      <c r="H40" s="36"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2605,15 +2638,15 @@
       <c r="C41" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="62" t="s">
+      <c r="D41" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="E41" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="73"/>
+      <c r="F41" s="91"/>
       <c r="G41" s="12"/>
-      <c r="H41" s="37"/>
+      <c r="H41" s="36"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2633,21 +2666,21 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" spans="1:26" s="8" customFormat="1" ht="51.6" customHeight="1">
+    <row r="42" spans="1:26" s="8" customFormat="1" ht="51.65" customHeight="1">
       <c r="A42" s="12"/>
       <c r="B42" s="19"/>
       <c r="C42" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="63" t="s">
+      <c r="D42" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="E42" s="30" t="s">
+      <c r="E42" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="73"/>
+      <c r="F42" s="91"/>
       <c r="G42" s="12"/>
-      <c r="H42" s="37"/>
+      <c r="H42" s="36"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -2671,15 +2704,15 @@
       <c r="A43" s="12"/>
       <c r="B43" s="19"/>
       <c r="C43" s="21"/>
-      <c r="D43" s="63" t="s">
+      <c r="D43" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="30" t="s">
+      <c r="E43" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="F43" s="73"/>
+      <c r="F43" s="91"/>
       <c r="G43" s="12"/>
-      <c r="H43" s="37"/>
+      <c r="H43" s="36"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -2699,21 +2732,21 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" s="8" customFormat="1" ht="67.2" customHeight="1">
+    <row r="44" spans="1:26" s="8" customFormat="1" ht="67.25" customHeight="1">
       <c r="A44" s="12"/>
       <c r="B44" s="19"/>
       <c r="C44" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="66" t="s">
+      <c r="D44" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="E44" s="30" t="s">
+      <c r="E44" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="74"/>
+      <c r="F44" s="92"/>
       <c r="G44" s="12"/>
-      <c r="H44" s="37"/>
+      <c r="H44" s="36"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -2739,13 +2772,13 @@
       <c r="C45" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="51"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="33" t="s">
+      <c r="D45" s="50"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="32" t="s">
         <v>78</v>
       </c>
       <c r="G45" s="12"/>
-      <c r="H45" s="37"/>
+      <c r="H45" s="36"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -2765,15 +2798,15 @@
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" spans="1:26" s="7" customFormat="1" ht="21.6" customHeight="1">
+    <row r="46" spans="1:26" s="7" customFormat="1" ht="21.65" customHeight="1">
       <c r="A46" s="16"/>
       <c r="B46" s="18"/>
       <c r="C46" s="22"/>
       <c r="D46" s="25"/>
       <c r="E46" s="18"/>
-      <c r="F46" s="34"/>
+      <c r="F46" s="33"/>
       <c r="G46" s="16"/>
-      <c r="H46" s="41"/>
+      <c r="H46" s="40"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -2794,28 +2827,28 @@
       <c r="Z46" s="6"/>
     </row>
     <row r="47" spans="1:26" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="75">
+      <c r="A47" s="71">
         <v>4</v>
       </c>
-      <c r="B47" s="78" t="s">
+      <c r="B47" s="74" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="81" t="s">
+      <c r="D47" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="E47" s="29" t="s">
+      <c r="E47" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F47" s="72" t="s">
+      <c r="F47" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="G47" s="37" t="s">
+      <c r="G47" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="H47" s="37"/>
+      <c r="H47" s="36"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -2836,18 +2869,18 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A48" s="76"/>
-      <c r="B48" s="79"/>
+      <c r="A48" s="72"/>
+      <c r="B48" s="75"/>
       <c r="C48" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="82"/>
-      <c r="E48" s="31" t="s">
+      <c r="D48" s="93"/>
+      <c r="E48" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="F48" s="73"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
+      <c r="F48" s="91"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -2868,16 +2901,16 @@
       <c r="Z48" s="9"/>
     </row>
     <row r="49" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A49" s="76"/>
-      <c r="B49" s="79"/>
+      <c r="A49" s="72"/>
+      <c r="B49" s="75"/>
       <c r="C49" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="82"/>
-      <c r="E49" s="86"/>
-      <c r="F49" s="73"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
+      <c r="D49" s="93"/>
+      <c r="E49" s="97"/>
+      <c r="F49" s="91"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -2898,14 +2931,14 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="76"/>
-      <c r="B50" s="79"/>
-      <c r="C50" s="84"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="87"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
+      <c r="A50" s="72"/>
+      <c r="B50" s="75"/>
+      <c r="C50" s="95"/>
+      <c r="D50" s="93"/>
+      <c r="E50" s="98"/>
+      <c r="F50" s="91"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -2926,14 +2959,14 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A51" s="77"/>
-      <c r="B51" s="80"/>
-      <c r="C51" s="85"/>
-      <c r="D51" s="83"/>
-      <c r="E51" s="88"/>
-      <c r="F51" s="74"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="37"/>
+      <c r="A51" s="73"/>
+      <c r="B51" s="76"/>
+      <c r="C51" s="96"/>
+      <c r="D51" s="94"/>
+      <c r="E51" s="99"/>
+      <c r="F51" s="92"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="36"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2953,15 +2986,15 @@
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
     </row>
-    <row r="52" spans="1:26" s="7" customFormat="1" ht="15.6" customHeight="1">
+    <row r="52" spans="1:26" s="7" customFormat="1" ht="15.65" customHeight="1">
       <c r="A52" s="16"/>
       <c r="B52" s="18"/>
       <c r="C52" s="22"/>
       <c r="D52" s="25"/>
       <c r="E52" s="18"/>
-      <c r="F52" s="34"/>
+      <c r="F52" s="33"/>
       <c r="G52" s="16"/>
-      <c r="H52" s="41"/>
+      <c r="H52" s="40"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -2981,27 +3014,27 @@
       <c r="Y52" s="6"/>
       <c r="Z52" s="6"/>
     </row>
-    <row r="53" spans="1:26" s="4" customFormat="1" ht="46.8" customHeight="1">
-      <c r="A53" s="92">
+    <row r="53" spans="1:26" s="4" customFormat="1" ht="46.75" customHeight="1">
+      <c r="A53" s="78">
         <v>5</v>
       </c>
-      <c r="B53" s="91" t="s">
+      <c r="B53" s="77" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="63" t="s">
+      <c r="D53" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="E53" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="F53" s="72" t="s">
+      <c r="F53" s="68" t="s">
         <v>90</v>
       </c>
       <c r="G53" s="12"/>
-      <c r="H53" s="37"/>
+      <c r="H53" s="36"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -3022,16 +3055,16 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="92"/>
-      <c r="B54" s="91"/>
+      <c r="A54" s="78"/>
+      <c r="B54" s="77"/>
       <c r="C54" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="27"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="96"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="37"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="36"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -3052,16 +3085,16 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A55" s="92"/>
-      <c r="B55" s="91"/>
+      <c r="A55" s="78"/>
+      <c r="B55" s="77"/>
       <c r="C55" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D55" s="27"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="97"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="70"/>
       <c r="G55" s="12"/>
-      <c r="H55" s="37"/>
+      <c r="H55" s="36"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -3081,15 +3114,15 @@
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
     </row>
-    <row r="56" spans="1:26" s="7" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="56" spans="1:26" s="7" customFormat="1" ht="18.649999999999999" customHeight="1">
       <c r="A56" s="16"/>
       <c r="B56" s="18"/>
       <c r="C56" s="22"/>
       <c r="D56" s="25"/>
       <c r="E56" s="18"/>
-      <c r="F56" s="34"/>
+      <c r="F56" s="33"/>
       <c r="G56" s="16"/>
-      <c r="H56" s="41"/>
+      <c r="H56" s="40"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -3110,24 +3143,24 @@
       <c r="Z56" s="6"/>
     </row>
     <row r="57" spans="1:26" s="4" customFormat="1" ht="21" customHeight="1">
-      <c r="A57" s="92">
+      <c r="A57" s="78">
         <v>6</v>
       </c>
-      <c r="B57" s="91" t="s">
+      <c r="B57" s="77" t="s">
         <v>35</v>
       </c>
       <c r="C57" s="23"/>
-      <c r="D57" s="101" t="s">
+      <c r="D57" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="E57" s="29" t="s">
+      <c r="E57" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F57" s="72" t="s">
+      <c r="F57" s="68" t="s">
         <v>92</v>
       </c>
       <c r="G57" s="12"/>
-      <c r="H57" s="37"/>
+      <c r="H57" s="36"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -3148,15 +3181,15 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" s="4" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A58" s="92"/>
-      <c r="B58" s="91"/>
-      <c r="D58" s="101"/>
-      <c r="E58" s="29" t="s">
+      <c r="A58" s="78"/>
+      <c r="B58" s="77"/>
+      <c r="D58" s="79"/>
+      <c r="E58" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="F58" s="96"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="37"/>
+      <c r="F58" s="69"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="36"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -3177,18 +3210,18 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" s="4" customFormat="1" ht="55.5" customHeight="1">
-      <c r="A59" s="92"/>
-      <c r="B59" s="91"/>
+      <c r="A59" s="78"/>
+      <c r="B59" s="77"/>
       <c r="C59" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="81"/>
-      <c r="E59" s="29" t="s">
+      <c r="D59" s="80"/>
+      <c r="E59" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="F59" s="97"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="37"/>
+      <c r="F59" s="70"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="36"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3209,18 +3242,18 @@
       <c r="Z59" s="3"/>
     </row>
     <row r="60" spans="1:26" s="8" customFormat="1" ht="47.4" customHeight="1">
-      <c r="A60" s="48"/>
-      <c r="B60" s="47"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="28" t="s">
+      <c r="A60" s="47"/>
+      <c r="B60" s="46"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="E60" s="49" t="s">
+      <c r="E60" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="F60" s="50"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="37"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="36"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -3240,19 +3273,19 @@
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" spans="1:26" s="8" customFormat="1" ht="69.599999999999994" customHeight="1">
-      <c r="A61" s="48"/>
-      <c r="B61" s="47"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="28" t="s">
+    <row r="61" spans="1:26" s="8" customFormat="1" ht="69.650000000000006" customHeight="1">
+      <c r="A61" s="47"/>
+      <c r="B61" s="46"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="E61" s="49" t="s">
+      <c r="E61" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="F61" s="50"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="37"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="36"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -3272,15 +3305,15 @@
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
     </row>
-    <row r="62" spans="1:26" s="7" customFormat="1" ht="22.95" customHeight="1">
+    <row r="62" spans="1:26" s="7" customFormat="1" ht="23" customHeight="1">
       <c r="A62" s="16"/>
       <c r="B62" s="18"/>
       <c r="C62" s="22"/>
       <c r="D62" s="25"/>
       <c r="E62" s="18"/>
-      <c r="F62" s="34"/>
+      <c r="F62" s="33"/>
       <c r="G62" s="16"/>
-      <c r="H62" s="41"/>
+      <c r="H62" s="40"/>
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
@@ -3300,7 +3333,7 @@
       <c r="Y62" s="6"/>
       <c r="Z62" s="6"/>
     </row>
-    <row r="63" spans="1:26" s="4" customFormat="1" ht="145.80000000000001" customHeight="1">
+    <row r="63" spans="1:26" s="4" customFormat="1" ht="145.75" customHeight="1">
       <c r="A63" s="12">
         <v>7</v>
       </c>
@@ -3310,19 +3343,19 @@
       <c r="C63" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D63" s="65" t="s">
+      <c r="D63" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="E63" s="32" t="s">
+      <c r="E63" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F63" s="35" t="s">
+      <c r="F63" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="G63" s="40" t="s">
+      <c r="G63" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="H63" s="37"/>
+      <c r="H63" s="36"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -3348,9 +3381,9 @@
       <c r="C64" s="22"/>
       <c r="D64" s="25"/>
       <c r="E64" s="18"/>
-      <c r="F64" s="34"/>
+      <c r="F64" s="33"/>
       <c r="G64" s="16"/>
-      <c r="H64" s="41"/>
+      <c r="H64" s="40"/>
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
@@ -3370,29 +3403,29 @@
       <c r="Y64" s="6"/>
       <c r="Z64" s="6"/>
     </row>
-    <row r="65" spans="1:26" s="4" customFormat="1" ht="75.599999999999994" customHeight="1">
-      <c r="A65" s="75">
+    <row r="65" spans="1:26" s="4" customFormat="1" ht="75.650000000000006" customHeight="1">
+      <c r="A65" s="71">
         <v>8</v>
       </c>
-      <c r="B65" s="78" t="s">
+      <c r="B65" s="74" t="s">
         <v>37</v>
       </c>
       <c r="C65" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D65" s="67" t="s">
+      <c r="D65" s="66" t="s">
         <v>135</v>
       </c>
       <c r="E65" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="72" t="s">
+      <c r="F65" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="G65" s="40" t="s">
+      <c r="G65" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="H65" s="37"/>
+      <c r="H65" s="36"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -3413,20 +3446,20 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A66" s="76"/>
-      <c r="B66" s="79"/>
+      <c r="A66" s="72"/>
+      <c r="B66" s="75"/>
       <c r="C66" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D66" s="67" t="s">
+      <c r="D66" s="66" t="s">
         <v>136</v>
       </c>
       <c r="E66" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="96"/>
-      <c r="G66" s="40"/>
-      <c r="H66" s="37"/>
+      <c r="F66" s="69"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="36"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -3447,20 +3480,20 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A67" s="76"/>
-      <c r="B67" s="79"/>
+      <c r="A67" s="72"/>
+      <c r="B67" s="75"/>
       <c r="C67" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D67" s="67" t="s">
+      <c r="D67" s="66" t="s">
         <v>137</v>
       </c>
       <c r="E67" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F67" s="96"/>
+      <c r="F67" s="69"/>
       <c r="G67" s="12"/>
-      <c r="H67" s="37"/>
+      <c r="H67" s="36"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -3481,14 +3514,14 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" s="4" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A68" s="77"/>
-      <c r="B68" s="80"/>
+      <c r="A68" s="73"/>
+      <c r="B68" s="76"/>
       <c r="C68" s="21"/>
-      <c r="D68" s="61"/>
+      <c r="D68" s="60"/>
       <c r="E68" s="20"/>
-      <c r="F68" s="97"/>
+      <c r="F68" s="70"/>
       <c r="G68" s="12"/>
-      <c r="H68" s="37"/>
+      <c r="H68" s="36"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -3508,15 +3541,15 @@
       <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
     </row>
-    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.2" customHeight="1">
+    <row r="69" spans="1:26" s="7" customFormat="1" ht="19.25" customHeight="1">
       <c r="A69" s="16"/>
       <c r="B69" s="18"/>
       <c r="C69" s="22"/>
       <c r="D69" s="25"/>
       <c r="E69" s="18"/>
-      <c r="F69" s="34"/>
+      <c r="F69" s="33"/>
       <c r="G69" s="16"/>
-      <c r="H69" s="41"/>
+      <c r="H69" s="40"/>
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
@@ -3536,7 +3569,7 @@
       <c r="Y69" s="6"/>
       <c r="Z69" s="6"/>
     </row>
-    <row r="70" spans="1:26" s="4" customFormat="1" ht="91.2" customHeight="1">
+    <row r="70" spans="1:26" s="4" customFormat="1" ht="91.25" customHeight="1">
       <c r="A70" s="12">
         <v>9</v>
       </c>
@@ -3544,17 +3577,17 @@
         <v>50</v>
       </c>
       <c r="C70" s="21"/>
-      <c r="D70" s="64" t="s">
+      <c r="D70" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="E70" s="30" t="s">
+      <c r="E70" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="F70" s="35" t="s">
+      <c r="F70" s="34" t="s">
         <v>93</v>
       </c>
       <c r="G70" s="12"/>
-      <c r="H70" s="37"/>
+      <c r="H70" s="36"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -3575,22 +3608,7 @@
       <c r="Z70" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="A11:A29"/>
-    <mergeCell ref="F11:F29"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="E21:E24"/>
+  <mergeCells count="33">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="F47:F51"/>
@@ -3607,6 +3625,23 @@
     <mergeCell ref="B11:B29"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A11:A29"/>
+    <mergeCell ref="F11:F29"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="D25:D32"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>